<commit_message>
Import file and Import Metadata bound to each other
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="171">
   <si>
     <t>Form Name</t>
   </si>
@@ -27,31 +27,94 @@
     <t>System Field</t>
   </si>
   <si>
-    <t>SR-Common</t>
+    <t>RegistrationEnrolmentAnnual</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>User File Type</t>
   </si>
   <si>
     <t>Registration</t>
   </si>
   <si>
-    <t>IndividualProfile</t>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Entity Type</t>
+  </si>
+  <si>
+    <t>Program Name</t>
+  </si>
+  <si>
+    <t>Encounter Type</t>
   </si>
   <si>
     <t>Registration Date</t>
   </si>
   <si>
+    <t>Date of Birth Verified</t>
+  </si>
+  <si>
+    <t>Enrolment Date</t>
+  </si>
+  <si>
+    <t>IndividualProfile</t>
+  </si>
+  <si>
+    <t>Actual Date</t>
+  </si>
+  <si>
+    <t>Test Import</t>
+  </si>
+  <si>
+    <t>Amalzar_Madhyamik_24-7</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
     <t>Sr No</t>
+  </si>
+  <si>
+    <t>Source User Field</t>
+  </si>
+  <si>
+    <t>Regex</t>
   </si>
   <si>
     <t>First Name</t>
   </si>
   <si>
-    <t>First Name Calculated</t>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>[a-zA-Z]+\s+[a-zA-Z]+</t>
   </si>
   <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>Last Name Calculated</t>
+    <t>[a-zA-Z]+\s+[a-zA-Z]+\s+([a-zA-Z]+).*</t>
+  </si>
+  <si>
+    <t>Father's Name</t>
+  </si>
+  <si>
+    <t>[a-zA-Z]+\s+([a-zA-Z]+).*</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ProgramEnrolment</t>
+  </si>
+  <si>
+    <t>Adolescent</t>
+  </si>
+  <si>
+    <t>ProgramEncounter</t>
   </si>
   <si>
     <t>Date of Birth</t>
@@ -60,7 +123,10 @@
     <t>DOB</t>
   </si>
   <si>
-    <t>Date of Birth Verified</t>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>Amalzar_Prathmik_3-8</t>
   </si>
   <si>
     <t>Gender</t>
@@ -69,19 +135,25 @@
     <t>Sex</t>
   </si>
   <si>
+    <t>Followup</t>
+  </si>
+  <si>
     <t>Village</t>
+  </si>
+  <si>
+    <t>Madhyamik_Follow up_26-9</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>ambos 3-10</t>
   </si>
   <si>
     <t>Mother's Name</t>
   </si>
   <si>
     <t>Mother'name</t>
-  </si>
-  <si>
-    <t>Father's Name</t>
-  </si>
-  <si>
-    <t>Father's Name Calculated</t>
   </si>
   <si>
     <t>Religion</t>
@@ -114,12 +186,6 @@
     <t>Adolescent Enrolment</t>
   </si>
   <si>
-    <t>ProgramEnrolment</t>
-  </si>
-  <si>
-    <t>Enrolment Date</t>
-  </si>
-  <si>
     <t>School going</t>
   </si>
   <si>
@@ -145,9 +211,6 @@
   </si>
   <si>
     <t>Adolescent School Dropout</t>
-  </si>
-  <si>
-    <t>ProgramEncounter</t>
   </si>
   <si>
     <t>Other reason according to teacher</t>
@@ -283,51 +346,6 @@
   </si>
   <si>
     <t>Is she slower than others in learning and understanding new things?</t>
-  </si>
-  <si>
-    <t>Unique Key</t>
-  </si>
-  <si>
-    <t>Source Field</t>
-  </si>
-  <si>
-    <t>Regex</t>
-  </si>
-  <si>
-    <t>File Name</t>
-  </si>
-  <si>
-    <t>User File Type</t>
-  </si>
-  <si>
-    <t>Sheet Name</t>
-  </si>
-  <si>
-    <t>Entity Type</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>Program Name</t>
-  </si>
-  <si>
-    <t>Encounter Type</t>
-  </si>
-  <si>
-    <t>1 Adol tracking_ Ambos.xlsx</t>
-  </si>
-  <si>
-    <t>ambos 3-10</t>
-  </si>
-  <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Adolescent</t>
   </si>
   <si>
     <t>Is there any developmental delay or disability seen?</t>
@@ -517,7 +535,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -534,6 +552,10 @@
     </font>
     <font>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -557,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -567,22 +589,25 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -619,7 +644,7 @@
     <col customWidth="1" min="2" max="2" width="19.14"/>
     <col customWidth="1" min="3" max="3" width="7.29"/>
     <col customWidth="1" min="4" max="4" width="43.0"/>
-    <col customWidth="1" min="5" max="5" width="20.57"/>
+    <col customWidth="1" min="5" max="5" width="29.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -655,20 +680,20 @@
       <c r="T1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="b">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -687,21 +712,19 @@
       <c r="T2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="b">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -719,21 +742,19 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="b">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="D4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="8"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -751,20 +772,20 @@
       <c r="T4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="b">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>14</v>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -783,19 +804,19 @@
       <c r="T5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="b">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -813,20 +834,20 @@
       <c r="T6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="b">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>17</v>
+      <c r="D7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -845,18 +866,18 @@
       <c r="T7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>18</v>
+      <c r="D8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -875,18 +896,18 @@
       <c r="T8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>20</v>
+      <c r="D9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -905,19 +926,17 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="6"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -935,17 +954,17 @@
       <c r="T10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="6"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -963,18 +982,18 @@
       <c r="T11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>25</v>
+      <c r="D12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -993,18 +1012,18 @@
       <c r="T12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>27</v>
+      <c r="D13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1023,18 +1042,18 @@
       <c r="T13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>29</v>
+      <c r="D14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1053,18 +1072,18 @@
       <c r="T14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>31</v>
+      <c r="D15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1083,19 +1102,19 @@
       <c r="T15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="3" t="b">
+      <c r="A16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1113,18 +1132,18 @@
       <c r="T16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
+      <c r="A17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>36</v>
+      <c r="D17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1143,17 +1162,17 @@
       <c r="T17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1171,17 +1190,17 @@
       <c r="T18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>38</v>
+      <c r="A19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="6"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1199,17 +1218,17 @@
       <c r="T19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>38</v>
+      <c r="A20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1227,17 +1246,17 @@
       <c r="T20" s="2"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>38</v>
+      <c r="A21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="6"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1255,17 +1274,17 @@
       <c r="T21" s="2"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>44</v>
+      <c r="A22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="4"/>
+      <c r="D22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="6"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1283,17 +1302,17 @@
       <c r="T22" s="2"/>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>44</v>
+      <c r="A23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="4"/>
+      <c r="D23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="6"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1311,17 +1330,17 @@
       <c r="T23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>44</v>
+      <c r="A24" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="4"/>
+      <c r="D24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1339,17 +1358,17 @@
       <c r="T24" s="2"/>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>44</v>
+      <c r="A25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="6"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1367,17 +1386,17 @@
       <c r="T25" s="2"/>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>44</v>
+      <c r="A26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="6"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1395,17 +1414,17 @@
       <c r="T26" s="2"/>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>44</v>
+      <c r="A27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="6"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1423,17 +1442,17 @@
       <c r="T27" s="2"/>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>44</v>
+      <c r="A28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1451,17 +1470,17 @@
       <c r="T28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>44</v>
+      <c r="A29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="6"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1479,18 +1498,18 @@
       <c r="T29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>44</v>
+      <c r="A30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>54</v>
+      <c r="D30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1509,18 +1528,18 @@
       <c r="T30" s="2"/>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>44</v>
+      <c r="A31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>56</v>
+      <c r="D31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1539,17 +1558,17 @@
       <c r="T31" s="2"/>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>44</v>
+      <c r="A32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="6"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1567,17 +1586,17 @@
       <c r="T32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>44</v>
+      <c r="A33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="6"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1595,18 +1614,18 @@
       <c r="T33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>44</v>
+      <c r="A34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>62</v>
+      <c r="D34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -1625,17 +1644,17 @@
       <c r="T34" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>44</v>
+      <c r="A35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" s="3"/>
+      <c r="D35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="4"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -1653,18 +1672,18 @@
       <c r="T35" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>44</v>
+      <c r="A36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>65</v>
+      <c r="D36" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1683,18 +1702,18 @@
       <c r="T36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>44</v>
+      <c r="A37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="D37" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>67</v>
+      <c r="D37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1713,17 +1732,17 @@
       <c r="T37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>44</v>
+      <c r="A38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C38" s="2"/>
-      <c r="D38" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="6"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1741,18 +1760,18 @@
       <c r="T38" s="2"/>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>44</v>
+      <c r="A39" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C39" s="2"/>
-      <c r="D39" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>69</v>
+      <c r="D39" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -1771,15 +1790,15 @@
       <c r="T39" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>44</v>
+      <c r="A40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="3" t="s">
-        <v>70</v>
+      <c r="D40" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1799,18 +1818,18 @@
       <c r="T40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>44</v>
+      <c r="A41" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>71</v>
+      <c r="D41" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -1829,18 +1848,18 @@
       <c r="T41" s="2"/>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>44</v>
+      <c r="A42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>72</v>
+      <c r="D42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -1859,18 +1878,18 @@
       <c r="T42" s="2"/>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>44</v>
+      <c r="A43" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>73</v>
+      <c r="D43" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -1889,18 +1908,18 @@
       <c r="T43" s="2"/>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>44</v>
+      <c r="A44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="D44" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>74</v>
+      <c r="D44" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -1919,18 +1938,18 @@
       <c r="T44" s="2"/>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>44</v>
+      <c r="A45" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C45" s="2"/>
-      <c r="D45" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>75</v>
+      <c r="D45" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -1949,18 +1968,18 @@
       <c r="T45" s="2"/>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>44</v>
+      <c r="A46" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>76</v>
+      <c r="D46" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -1979,18 +1998,18 @@
       <c r="T46" s="2"/>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>44</v>
+      <c r="A47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>77</v>
+      <c r="D47" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -2009,18 +2028,18 @@
       <c r="T47" s="2"/>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>44</v>
+      <c r="A48" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>78</v>
+      <c r="D48" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -2039,18 +2058,18 @@
       <c r="T48" s="2"/>
     </row>
     <row r="49">
-      <c r="A49" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>44</v>
+      <c r="A49" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C49" s="2"/>
-      <c r="D49" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>79</v>
+      <c r="D49" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -2069,18 +2088,18 @@
       <c r="T49" s="2"/>
     </row>
     <row r="50">
-      <c r="A50" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>44</v>
+      <c r="A50" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>80</v>
+      <c r="D50" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -2099,18 +2118,18 @@
       <c r="T50" s="2"/>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>44</v>
+      <c r="A51" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>81</v>
+      <c r="D51" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -2129,18 +2148,18 @@
       <c r="T51" s="2"/>
     </row>
     <row r="52">
-      <c r="A52" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>44</v>
+      <c r="A52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>82</v>
+      <c r="D52" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -2159,18 +2178,18 @@
       <c r="T52" s="2"/>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>44</v>
+      <c r="A53" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>83</v>
+      <c r="D53" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -2189,18 +2208,18 @@
       <c r="T53" s="2"/>
     </row>
     <row r="54">
-      <c r="A54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>44</v>
+      <c r="A54" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C54" s="2"/>
-      <c r="D54" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>84</v>
+      <c r="D54" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -2219,15 +2238,15 @@
       <c r="T54" s="2"/>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>44</v>
+      <c r="A55" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C55" s="2"/>
-      <c r="D55" s="3" t="s">
-        <v>85</v>
+      <c r="D55" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
@@ -2247,18 +2266,18 @@
       <c r="T55" s="2"/>
     </row>
     <row r="56">
-      <c r="A56" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>44</v>
+      <c r="A56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="D56" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>86</v>
+      <c r="D56" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -2277,18 +2296,18 @@
       <c r="T56" s="2"/>
     </row>
     <row r="57">
-      <c r="A57" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>44</v>
+      <c r="A57" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C57" s="2"/>
-      <c r="D57" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>87</v>
+      <c r="D57" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -2307,18 +2326,18 @@
       <c r="T57" s="2"/>
     </row>
     <row r="58">
-      <c r="A58" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>44</v>
+      <c r="A58" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C58" s="2"/>
-      <c r="D58" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>88</v>
+      <c r="D58" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -2337,18 +2356,18 @@
       <c r="T58" s="2"/>
     </row>
     <row r="59">
-      <c r="A59" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>44</v>
+      <c r="A59" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C59" s="2"/>
-      <c r="D59" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>89</v>
+      <c r="D59" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -2367,18 +2386,18 @@
       <c r="T59" s="2"/>
     </row>
     <row r="60">
-      <c r="A60" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>44</v>
+      <c r="A60" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C60" s="2"/>
-      <c r="D60" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>105</v>
+      <c r="D60" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -2397,18 +2416,18 @@
       <c r="T60" s="2"/>
     </row>
     <row r="61">
-      <c r="A61" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>44</v>
+      <c r="A61" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>107</v>
+      <c r="D61" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -2427,18 +2446,18 @@
       <c r="T61" s="2"/>
     </row>
     <row r="62">
-      <c r="A62" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>44</v>
+      <c r="A62" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C62" s="2"/>
-      <c r="D62" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>109</v>
+      <c r="D62" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -2457,18 +2476,18 @@
       <c r="T62" s="2"/>
     </row>
     <row r="63">
-      <c r="A63" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>44</v>
+      <c r="A63" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C63" s="2"/>
-      <c r="D63" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>110</v>
+      <c r="D63" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -2487,18 +2506,18 @@
       <c r="T63" s="2"/>
     </row>
     <row r="64">
-      <c r="A64" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>44</v>
+      <c r="A64" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C64" s="2"/>
-      <c r="D64" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>112</v>
+      <c r="D64" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -2517,18 +2536,18 @@
       <c r="T64" s="2"/>
     </row>
     <row r="65">
-      <c r="A65" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>44</v>
+      <c r="A65" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C65" s="2"/>
-      <c r="D65" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>113</v>
+      <c r="D65" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -2547,18 +2566,18 @@
       <c r="T65" s="2"/>
     </row>
     <row r="66">
-      <c r="A66" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>44</v>
+      <c r="A66" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C66" s="2"/>
-      <c r="D66" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>114</v>
+      <c r="D66" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -2577,18 +2596,18 @@
       <c r="T66" s="2"/>
     </row>
     <row r="67">
-      <c r="A67" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>44</v>
+      <c r="A67" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C67" s="2"/>
-      <c r="D67" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>116</v>
+      <c r="D67" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2607,17 +2626,17 @@
       <c r="T67" s="2"/>
     </row>
     <row r="68">
-      <c r="A68" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>44</v>
+      <c r="A68" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C68" s="2"/>
-      <c r="D68" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E68" s="4"/>
+      <c r="D68" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68" s="6"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
@@ -2635,17 +2654,17 @@
       <c r="T68" s="2"/>
     </row>
     <row r="69">
-      <c r="A69" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>44</v>
+      <c r="A69" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C69" s="2"/>
-      <c r="D69" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E69" s="4"/>
+      <c r="D69" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E69" s="6"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -2663,18 +2682,18 @@
       <c r="T69" s="2"/>
     </row>
     <row r="70">
-      <c r="A70" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>44</v>
+      <c r="A70" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C70" s="2"/>
-      <c r="D70" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>119</v>
+      <c r="D70" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -2693,17 +2712,17 @@
       <c r="T70" s="2"/>
     </row>
     <row r="71">
-      <c r="A71" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>44</v>
+      <c r="A71" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C71" s="2"/>
-      <c r="D71" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E71" s="4"/>
+      <c r="D71" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E71" s="6"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -2721,18 +2740,18 @@
       <c r="T71" s="2"/>
     </row>
     <row r="72">
-      <c r="A72" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>44</v>
+      <c r="A72" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C72" s="2"/>
-      <c r="D72" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>121</v>
+      <c r="D72" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -2751,15 +2770,15 @@
       <c r="T72" s="2"/>
     </row>
     <row r="73">
-      <c r="A73" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>44</v>
+      <c r="A73" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C73" s="2"/>
-      <c r="D73" s="3" t="s">
-        <v>122</v>
+      <c r="D73" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2779,18 +2798,18 @@
       <c r="T73" s="2"/>
     </row>
     <row r="74">
-      <c r="A74" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>44</v>
+      <c r="A74" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C74" s="2"/>
-      <c r="D74" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>123</v>
+      <c r="D74" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -2809,18 +2828,18 @@
       <c r="T74" s="2"/>
     </row>
     <row r="75">
-      <c r="A75" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>44</v>
+      <c r="A75" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C75" s="2"/>
-      <c r="D75" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>125</v>
+      <c r="D75" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
@@ -2839,18 +2858,18 @@
       <c r="T75" s="2"/>
     </row>
     <row r="76">
-      <c r="A76" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>44</v>
+      <c r="A76" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C76" s="2"/>
-      <c r="D76" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>127</v>
+      <c r="D76" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -2869,18 +2888,18 @@
       <c r="T76" s="2"/>
     </row>
     <row r="77">
-      <c r="A77" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>44</v>
+      <c r="A77" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C77" s="2"/>
-      <c r="D77" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>128</v>
+      <c r="D77" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -2899,18 +2918,18 @@
       <c r="T77" s="2"/>
     </row>
     <row r="78">
-      <c r="A78" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>44</v>
+      <c r="A78" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C78" s="2"/>
-      <c r="D78" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>129</v>
+      <c r="D78" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -2929,18 +2948,18 @@
       <c r="T78" s="2"/>
     </row>
     <row r="79">
-      <c r="A79" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>44</v>
+      <c r="A79" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C79" s="2"/>
-      <c r="D79" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>130</v>
+      <c r="D79" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -2959,15 +2978,15 @@
       <c r="T79" s="2"/>
     </row>
     <row r="80">
-      <c r="A80" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>44</v>
+      <c r="A80" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C80" s="2"/>
-      <c r="D80" s="3" t="s">
-        <v>131</v>
+      <c r="D80" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -2987,15 +3006,15 @@
       <c r="T80" s="2"/>
     </row>
     <row r="81">
-      <c r="A81" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>44</v>
+      <c r="A81" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C81" s="2"/>
-      <c r="D81" s="3" t="s">
-        <v>132</v>
+      <c r="D81" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -3015,15 +3034,15 @@
       <c r="T81" s="2"/>
     </row>
     <row r="82">
-      <c r="A82" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>44</v>
+      <c r="A82" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C82" s="2"/>
-      <c r="D82" s="3" t="s">
-        <v>133</v>
+      <c r="D82" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -3043,18 +3062,18 @@
       <c r="T82" s="2"/>
     </row>
     <row r="83">
-      <c r="A83" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>44</v>
+      <c r="A83" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C83" s="2"/>
-      <c r="D83" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>135</v>
+      <c r="D83" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -3073,18 +3092,18 @@
       <c r="T83" s="2"/>
     </row>
     <row r="84">
-      <c r="A84" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>44</v>
+      <c r="A84" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C84" s="2"/>
-      <c r="D84" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>137</v>
+      <c r="D84" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>143</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -3103,18 +3122,18 @@
       <c r="T84" s="2"/>
     </row>
     <row r="85">
-      <c r="A85" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>44</v>
+      <c r="A85" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C85" s="2"/>
-      <c r="D85" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>139</v>
+      <c r="D85" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -3133,15 +3152,15 @@
       <c r="T85" s="2"/>
     </row>
     <row r="86">
-      <c r="A86" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>44</v>
+      <c r="A86" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C86" s="2"/>
-      <c r="D86" s="3" t="s">
-        <v>140</v>
+      <c r="D86" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
@@ -3161,18 +3180,18 @@
       <c r="T86" s="2"/>
     </row>
     <row r="87">
-      <c r="A87" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>44</v>
+      <c r="A87" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C87" s="2"/>
-      <c r="D87" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>142</v>
+      <c r="D87" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -3191,15 +3210,15 @@
       <c r="T87" s="2"/>
     </row>
     <row r="88">
-      <c r="A88" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>44</v>
+      <c r="A88" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C88" s="2"/>
-      <c r="D88" s="3" t="s">
-        <v>143</v>
+      <c r="D88" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -3219,15 +3238,15 @@
       <c r="T88" s="2"/>
     </row>
     <row r="89">
-      <c r="A89" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>44</v>
+      <c r="A89" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C89" s="2"/>
-      <c r="D89" s="3" t="s">
-        <v>144</v>
+      <c r="D89" s="4" t="s">
+        <v>150</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
@@ -3247,15 +3266,15 @@
       <c r="T89" s="2"/>
     </row>
     <row r="90">
-      <c r="A90" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>44</v>
+      <c r="A90" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C90" s="2"/>
-      <c r="D90" s="3" t="s">
-        <v>35</v>
+      <c r="D90" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
@@ -3275,15 +3294,15 @@
       <c r="T90" s="2"/>
     </row>
     <row r="91">
-      <c r="A91" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>44</v>
+      <c r="A91" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C91" s="2"/>
-      <c r="D91" s="3" t="s">
-        <v>50</v>
+      <c r="D91" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -3303,18 +3322,18 @@
       <c r="T91" s="2"/>
     </row>
     <row r="92">
-      <c r="A92" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>44</v>
+      <c r="A92" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C92" s="2"/>
-      <c r="D92" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>146</v>
+      <c r="D92" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -3333,18 +3352,18 @@
       <c r="T92" s="2"/>
     </row>
     <row r="93">
-      <c r="A93" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>44</v>
+      <c r="A93" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C93" s="2"/>
-      <c r="D93" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>148</v>
+      <c r="D93" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -3363,18 +3382,18 @@
       <c r="T93" s="2"/>
     </row>
     <row r="94">
-      <c r="A94" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>44</v>
+      <c r="A94" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C94" s="2"/>
-      <c r="D94" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>150</v>
+      <c r="D94" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3393,18 +3412,18 @@
       <c r="T94" s="2"/>
     </row>
     <row r="95">
-      <c r="A95" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>44</v>
+      <c r="A95" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C95" s="2"/>
-      <c r="D95" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>152</v>
+      <c r="D95" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -3423,18 +3442,18 @@
       <c r="T95" s="2"/>
     </row>
     <row r="96">
-      <c r="A96" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>44</v>
+      <c r="A96" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C96" s="2"/>
-      <c r="D96" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>154</v>
+      <c r="D96" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -3453,15 +3472,15 @@
       <c r="T96" s="2"/>
     </row>
     <row r="97">
-      <c r="A97" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>44</v>
+      <c r="A97" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C97" s="2"/>
-      <c r="D97" s="3" t="s">
-        <v>155</v>
+      <c r="D97" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
@@ -3481,18 +3500,18 @@
       <c r="T97" s="2"/>
     </row>
     <row r="98">
-      <c r="A98" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>44</v>
+      <c r="A98" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C98" s="2"/>
-      <c r="D98" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E98" s="4" t="s">
-        <v>156</v>
+      <c r="D98" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -3511,18 +3530,18 @@
       <c r="T98" s="2"/>
     </row>
     <row r="99">
-      <c r="A99" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>44</v>
+      <c r="A99" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C99" s="2"/>
-      <c r="D99" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>157</v>
+      <c r="D99" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -3541,18 +3560,18 @@
       <c r="T99" s="2"/>
     </row>
     <row r="100">
-      <c r="A100" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>44</v>
+      <c r="A100" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C100" s="2"/>
-      <c r="D100" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>159</v>
+      <c r="D100" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -3571,18 +3590,18 @@
       <c r="T100" s="2"/>
     </row>
     <row r="101">
-      <c r="A101" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>44</v>
+      <c r="A101" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C101" s="2"/>
-      <c r="D101" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>160</v>
+      <c r="D101" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -3601,18 +3620,18 @@
       <c r="T101" s="2"/>
     </row>
     <row r="102">
-      <c r="A102" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>44</v>
+      <c r="A102" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C102" s="2"/>
-      <c r="D102" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>161</v>
+      <c r="D102" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -3631,18 +3650,18 @@
       <c r="T102" s="2"/>
     </row>
     <row r="103">
-      <c r="A103" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>44</v>
+      <c r="A103" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C103" s="2"/>
-      <c r="D103" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>162</v>
+      <c r="D103" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -3661,18 +3680,18 @@
       <c r="T103" s="2"/>
     </row>
     <row r="104">
-      <c r="A104" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>44</v>
+      <c r="A104" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C104" s="2"/>
-      <c r="D104" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>163</v>
+      <c r="D104" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
@@ -3691,15 +3710,15 @@
       <c r="T104" s="2"/>
     </row>
     <row r="105">
-      <c r="A105" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>44</v>
+      <c r="A105" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C105" s="2"/>
-      <c r="D105" s="3" t="s">
-        <v>164</v>
+      <c r="D105" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -18866,68 +18885,83 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.57"/>
-    <col customWidth="1" min="3" max="4" width="18.14"/>
+    <col customWidth="1" min="1" max="1" width="25.29"/>
+    <col customWidth="1" min="2" max="4" width="18.14"/>
+    <col customWidth="1" min="5" max="5" width="31.71"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>97</v>
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>97</v>
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>97</v>
-      </c>
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -18941,8 +18975,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="25.57"/>
-    <col customWidth="1" min="3" max="3" width="18.14"/>
+    <col customWidth="1" min="1" max="1" width="25.57"/>
+    <col customWidth="1" min="2" max="2" width="27.0"/>
+    <col customWidth="1" min="3" max="3" width="24.43"/>
     <col customWidth="1" min="4" max="4" width="16.71"/>
     <col customWidth="1" min="6" max="7" width="18.14"/>
     <col customWidth="1" min="8" max="8" width="19.57"/>
@@ -18950,91 +18985,264 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>34</v>
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="G2" s="8">
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="G2" s="7">
+        <v>42940.0</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="7">
+        <v>42940.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="7">
+        <v>42940.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="G5" s="7">
+        <v>42950.0</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="7">
+        <v>42950.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="5"/>
+      <c r="J7" s="7">
+        <v>42950.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="7">
+        <v>43004.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="7">
         <v>43011.0</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="H9" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="C10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="7">
+        <v>43011.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8">
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="7">
         <v>43011.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing tests whilst adding new address field to sheet metadata
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -1,20 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/projects/work/openchs/openchs-server/openchs-server-api/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Fields" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Answer Fields" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Calculated Fields" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheets" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Fields" sheetId="1" r:id="rId1"/>
+    <sheet name="Answer Fields" sheetId="2" r:id="rId2"/>
+    <sheet name="Calculated Fields" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheets" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -23,716 +33,702 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="207">
-  <si>
-    <t xml:space="preserve">Form Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Form Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Core</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegistrationEnrolmentAnnualSchool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegistrationEnrolmentAnnualVillage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IndividualProfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registration Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of Birth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of Birth Verified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother's Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father's Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Religion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caste Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aadhar ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique health ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ration Card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ration card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact Number 1:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adolescent Enrolment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramEnrolment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enrolment Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School going</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adol education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adolescent Exit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramExit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adolescent exit reason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unspecified Cause of Death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cause of Death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age at Marriage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adolescent School Dropout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ProgramEncounter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other reason according to teacher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What he/she is doing now?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is she/he doing?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How is the economic condition of family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are you ready for re-admission to school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other reason according to student/parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When did you leave school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dropped out of which standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If not in School (dropped out) After which standard left the school:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reason for dropping as per student / parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If not in school (dropped out) Reasons for dropping out:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reason for dropping as per teacher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adolescent School Dropout Followup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have you started going to school once again</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Routine Visit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hemoglobin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sickling Test Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sickling Test Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sickling (If HB&lt;7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron tablets received</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron tablets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron tablets provider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron tablets consumed in last month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Albendazole tablets received?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any physical defect?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there a swelling at lower back?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there Cleft lip/Cleft palate?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there large gap between toe and finger?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is her nails/tongue pale?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is she/he severely malnourished?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any problem in leg bone?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there a swelling over throat?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does she have difficulty in breathing while playing?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are there dental carries?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there a white patch in her eyes?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does she have impaired vision?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there pus coming from ear?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does she have impaired hearing?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does she have skin problems?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has she ever suffered from convulsions?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any neurological motor defect?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is her behavior different from others?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is she slower than others in learning and understanding new things?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any developmental delay or disability seen?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menstruation started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menstrutation started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age when menstruation started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If Yes, Age at Menarche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absorbent material used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menstrual disorders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menstrual disorder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any treatment taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does she remain absent during menstruation?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reason for remaining absent during menstruation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If yes reason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other reason for remaining absent during menstruation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How many days does she take off during menstruation?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any other condition you want to mention about him/her?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other conditions mentioned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sickness in last 3 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other sickness in last 3 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitalized in last 3 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addiction Details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have any addiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are friends addicted?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How are your friends?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sexually active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unprotected sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple Sexual Partners</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partners</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burning Micturition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ulcer over genitalia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellowish discharge from Vagina / penis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owns 2 wheeler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vehicle (2 wheeler)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drives 2 wheeler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you drive 2 wheeler?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has driving license</t>
-  </si>
-  <si>
-    <t xml:space="preserve">License</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wears helmet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Road accident in past 6 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Have you suffered from Road Traffic Accident in last 6 months?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How the accident has happened?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Counselling for Severe Anemia Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parents' life status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father's Occupation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father's occupation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father's Addiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father's addiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother's Occupation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother's occupation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother's Addiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother's addiction (Alcohol)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Staying with</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of brothers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of sisters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Sisters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chronic sickness in family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BMI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hemoglobin Test Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Continued</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dropped Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discountinued</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not received</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Received</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nausea and vomiting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nausea-vomiting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addicted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Friend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No frnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not applicable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No treatment taken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No treatment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consulted doctor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doctor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Job</t>
-  </si>
-  <si>
-    <t xml:space="preserve">job</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only Mother Alive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only Mother alive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only Father Alive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Only Father alive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User File Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entity Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source User Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[a-zA-Z]+\s+[a-zA-Z]+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[a-zA-Z]+\s+[a-zA-Z]+\s+([a-zA-Z]+).*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[a-zA-Z]+\s+([a-zA-Z]+).*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.*(\d).*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sheet Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Program Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visit Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amalzar_Madhyamik_24-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adolescent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amalzar_Prathmik_3-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Followup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Madhyamik_Follow up_26-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ambos 3-10</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="211">
+  <si>
+    <t>Form Name</t>
+  </si>
+  <si>
+    <t>Form Type</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>System Field</t>
+  </si>
+  <si>
+    <t>RegistrationEnrolmentAnnualSchool</t>
+  </si>
+  <si>
+    <t>RegistrationEnrolmentAnnualVillage</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>IndividualProfile</t>
+  </si>
+  <si>
+    <t>Registration Date</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Date of Birth Verified</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Mother's Name</t>
+  </si>
+  <si>
+    <t>Father's Name</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Caste Category</t>
+  </si>
+  <si>
+    <t>Cast</t>
+  </si>
+  <si>
+    <t>Aadhar ID</t>
+  </si>
+  <si>
+    <t>Unique health ID</t>
+  </si>
+  <si>
+    <t>Ration Card</t>
+  </si>
+  <si>
+    <t>Ration card</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Contact Number 1:</t>
+  </si>
+  <si>
+    <t>Adolescent Enrolment</t>
+  </si>
+  <si>
+    <t>ProgramEnrolment</t>
+  </si>
+  <si>
+    <t>Enrolment Date</t>
+  </si>
+  <si>
+    <t>School going</t>
+  </si>
+  <si>
+    <t>Adol education</t>
+  </si>
+  <si>
+    <t>Adolescent Exit</t>
+  </si>
+  <si>
+    <t>ProgramExit</t>
+  </si>
+  <si>
+    <t>Adolescent exit reason</t>
+  </si>
+  <si>
+    <t>Unspecified Cause of Death</t>
+  </si>
+  <si>
+    <t>Cause of Death</t>
+  </si>
+  <si>
+    <t>Age at Marriage</t>
+  </si>
+  <si>
+    <t>Adolescent School Dropout</t>
+  </si>
+  <si>
+    <t>ProgramEncounter</t>
+  </si>
+  <si>
+    <t>Other reason according to teacher</t>
+  </si>
+  <si>
+    <t>What he/she is doing now?</t>
+  </si>
+  <si>
+    <t>What is she/he doing?</t>
+  </si>
+  <si>
+    <t>Other activity</t>
+  </si>
+  <si>
+    <t>How is the economic condition of family</t>
+  </si>
+  <si>
+    <t>Are you ready for re-admission to school</t>
+  </si>
+  <si>
+    <t>Name of school</t>
+  </si>
+  <si>
+    <t>Other reason according to student/parent</t>
+  </si>
+  <si>
+    <t>When did you leave school</t>
+  </si>
+  <si>
+    <t>Dropped out of which standard</t>
+  </si>
+  <si>
+    <t>If not in School (dropped out) After which standard left the school:</t>
+  </si>
+  <si>
+    <t>Reason for dropping as per student / parent</t>
+  </si>
+  <si>
+    <t>If not in school (dropped out) Reasons for dropping out:</t>
+  </si>
+  <si>
+    <t>Reason for dropping as per teacher</t>
+  </si>
+  <si>
+    <t>Adolescent School Dropout Followup</t>
+  </si>
+  <si>
+    <t>Have you started going to school once again</t>
+  </si>
+  <si>
+    <t>Routine Visit</t>
+  </si>
+  <si>
+    <t>Hb</t>
+  </si>
+  <si>
+    <t>Hemoglobin</t>
+  </si>
+  <si>
+    <t>Sickling Test Done</t>
+  </si>
+  <si>
+    <t>Sickling Test Result</t>
+  </si>
+  <si>
+    <t>Sickling (If HB&lt;7)</t>
+  </si>
+  <si>
+    <t>Iron tablets received</t>
+  </si>
+  <si>
+    <t>Iron tablets</t>
+  </si>
+  <si>
+    <t>Iron tablets provider</t>
+  </si>
+  <si>
+    <t>Iron tablets consumed in last month</t>
+  </si>
+  <si>
+    <t>Albendazole tablets received?</t>
+  </si>
+  <si>
+    <t>Is there any physical defect?</t>
+  </si>
+  <si>
+    <t>Is there a swelling at lower back?</t>
+  </si>
+  <si>
+    <t>Is there Cleft lip/Cleft palate?</t>
+  </si>
+  <si>
+    <t>Is there large gap between toe and finger?</t>
+  </si>
+  <si>
+    <t>Is her nails/tongue pale?</t>
+  </si>
+  <si>
+    <t>Is she/he severely malnourished?</t>
+  </si>
+  <si>
+    <t>Is there any problem in leg bone?</t>
+  </si>
+  <si>
+    <t>Is there a swelling over throat?</t>
+  </si>
+  <si>
+    <t>Does she have difficulty in breathing while playing?</t>
+  </si>
+  <si>
+    <t>Are there dental carries?</t>
+  </si>
+  <si>
+    <t>Is there a white patch in her eyes?</t>
+  </si>
+  <si>
+    <t>Does she have impaired vision?</t>
+  </si>
+  <si>
+    <t>Is there pus coming from ear?</t>
+  </si>
+  <si>
+    <t>Does she have impaired hearing?</t>
+  </si>
+  <si>
+    <t>Does she have skin problems?</t>
+  </si>
+  <si>
+    <t>Has she ever suffered from convulsions?</t>
+  </si>
+  <si>
+    <t>Is there any neurological motor defect?</t>
+  </si>
+  <si>
+    <t>Is her behavior different from others?</t>
+  </si>
+  <si>
+    <t>Is she slower than others in learning and understanding new things?</t>
+  </si>
+  <si>
+    <t>Is there any developmental delay or disability seen?</t>
+  </si>
+  <si>
+    <t>Menstruation started</t>
+  </si>
+  <si>
+    <t>Menstrutation started</t>
+  </si>
+  <si>
+    <t>Age when menstruation started</t>
+  </si>
+  <si>
+    <t>If Yes, Age at Menarche</t>
+  </si>
+  <si>
+    <t>Absorbent material used</t>
+  </si>
+  <si>
+    <t>Menstrual disorders</t>
+  </si>
+  <si>
+    <t>Menstrual disorder</t>
+  </si>
+  <si>
+    <t>Any treatment taken</t>
+  </si>
+  <si>
+    <t>Does she remain absent during menstruation?</t>
+  </si>
+  <si>
+    <t>Reason for remaining absent during menstruation</t>
+  </si>
+  <si>
+    <t>If yes reason</t>
+  </si>
+  <si>
+    <t>Other reason for remaining absent during menstruation</t>
+  </si>
+  <si>
+    <t>How many days does she take off during menstruation?</t>
+  </si>
+  <si>
+    <t>Is there any other condition you want to mention about him/her?</t>
+  </si>
+  <si>
+    <t>Other conditions mentioned</t>
+  </si>
+  <si>
+    <t>Sickness in last 3 months</t>
+  </si>
+  <si>
+    <t>Other sickness in last 3 months</t>
+  </si>
+  <si>
+    <t>Hospitalized in last 3 months</t>
+  </si>
+  <si>
+    <t>Addiction Details</t>
+  </si>
+  <si>
+    <t>Do you have any addiction</t>
+  </si>
+  <si>
+    <t>Are friends addicted?</t>
+  </si>
+  <si>
+    <t>How are your friends?</t>
+  </si>
+  <si>
+    <t>Sexually active</t>
+  </si>
+  <si>
+    <t>Unprotected sex</t>
+  </si>
+  <si>
+    <t>Multiple Sexual Partners</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>Burning Micturition</t>
+  </si>
+  <si>
+    <t>Ulcer over genitalia</t>
+  </si>
+  <si>
+    <t>Yellowish discharge from Vagina / penis</t>
+  </si>
+  <si>
+    <t>Owns 2 wheeler</t>
+  </si>
+  <si>
+    <t>Vehicle (2 wheeler)</t>
+  </si>
+  <si>
+    <t>Drives 2 wheeler</t>
+  </si>
+  <si>
+    <t>Do you drive 2 wheeler?</t>
+  </si>
+  <si>
+    <t>Has driving license</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>Wears helmet</t>
+  </si>
+  <si>
+    <t>Road accident in past 6 months</t>
+  </si>
+  <si>
+    <t>Have you suffered from Road Traffic Accident in last 6 months?</t>
+  </si>
+  <si>
+    <t>How the accident has happened?</t>
+  </si>
+  <si>
+    <t>Counselling for Severe Anemia Done</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Parents' life status</t>
+  </si>
+  <si>
+    <t>Parents</t>
+  </si>
+  <si>
+    <t>Father's Occupation</t>
+  </si>
+  <si>
+    <t>Father's occupation</t>
+  </si>
+  <si>
+    <t>Father's Addiction</t>
+  </si>
+  <si>
+    <t>Father's addiction</t>
+  </si>
+  <si>
+    <t>Mother's Occupation</t>
+  </si>
+  <si>
+    <t>Mother's occupation</t>
+  </si>
+  <si>
+    <t>Mother's Addiction</t>
+  </si>
+  <si>
+    <t>Mother's addiction (Alcohol)</t>
+  </si>
+  <si>
+    <t>Staying with</t>
+  </si>
+  <si>
+    <t>Number of brothers</t>
+  </si>
+  <si>
+    <t>Number of sisters</t>
+  </si>
+  <si>
+    <t>Number of Sisters</t>
+  </si>
+  <si>
+    <t>Chronic sickness in family</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>Hemoglobin Test Done</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>System Answer</t>
+  </si>
+  <si>
+    <t>User Answer</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Continued</t>
+  </si>
+  <si>
+    <t>Dropped Out</t>
+  </si>
+  <si>
+    <t>Discountinued</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Not received</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>Nausea and vomiting</t>
+  </si>
+  <si>
+    <t>Nausea-vomiting</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Addicted</t>
+  </si>
+  <si>
+    <t>No Friend</t>
+  </si>
+  <si>
+    <t>No frnd</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>No treatment taken</t>
+  </si>
+  <si>
+    <t>No treatment</t>
+  </si>
+  <si>
+    <t>Consulted doctor</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>job</t>
+  </si>
+  <si>
+    <t>Only Mother Alive</t>
+  </si>
+  <si>
+    <t>Only Mother alive</t>
+  </si>
+  <si>
+    <t>Only Father Alive</t>
+  </si>
+  <si>
+    <t>Only Father alive</t>
+  </si>
+  <si>
+    <t>User File Type</t>
+  </si>
+  <si>
+    <t>Entity Type</t>
+  </si>
+  <si>
+    <t>Source User Field</t>
+  </si>
+  <si>
+    <t>Regex</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>[a-zA-Z]+\s+[a-zA-Z]+</t>
+  </si>
+  <si>
+    <t>[a-zA-Z]+\s+[a-zA-Z]+\s+([a-zA-Z]+).*</t>
+  </si>
+  <si>
+    <t>[a-zA-Z]+\s+([a-zA-Z]+).*</t>
+  </si>
+  <si>
+    <t>.*(\d).*</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Program Name</t>
+  </si>
+  <si>
+    <t>Visit Type</t>
+  </si>
+  <si>
+    <t>Actual Date</t>
+  </si>
+  <si>
+    <t>Test Import</t>
+  </si>
+  <si>
+    <t>Amalzar_Madhyamik_24-7</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Adolescent</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>Amalzar_Prathmik_3-8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Followup</t>
+  </si>
+  <si>
+    <t>Madhyamik_Follow up_26-9</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>ambos 3-10</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Amalzar Secondary</t>
+  </si>
+  <si>
+    <t>Amalzar Primary</t>
+  </si>
+  <si>
+    <t>Aambos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
-    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -751,7 +747,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -759,101 +755,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -912,36 +850,306 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF222222"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F89" activeCellId="0" sqref="F89"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.43"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:20" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,15 +1183,15 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C2" s="3" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1006,15 +1214,15 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C3" s="3" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1037,15 +1245,15 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C4" s="3" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1068,15 +1276,15 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C5" s="3" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1103,15 +1311,15 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C6" s="3" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1134,15 +1342,15 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C7" s="3" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1169,7 +1377,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1201,7 +1409,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1233,7 +1441,7 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1261,7 +1469,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1289,7 +1497,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1321,7 +1529,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1353,7 +1561,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1385,7 +1593,7 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1417,15 +1625,15 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="3" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="C16" s="3" t="b">
+        <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -1448,7 +1656,7 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1480,7 +1688,7 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -1508,7 +1716,7 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1536,7 +1744,7 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1564,7 +1772,7 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -1592,7 +1800,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
@@ -1620,7 +1828,7 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
@@ -1652,7 +1860,7 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1680,7 +1888,7 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>39</v>
       </c>
@@ -1708,7 +1916,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -1736,7 +1944,7 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
@@ -1764,7 +1972,7 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
@@ -1792,7 +2000,7 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -1820,7 +2028,7 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -1852,7 +2060,7 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1884,7 +2092,7 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -1912,7 +2120,7 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
@@ -1940,7 +2148,7 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>57</v>
       </c>
@@ -1972,7 +2180,7 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -2000,7 +2208,7 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
@@ -2032,7 +2240,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -2064,7 +2272,7 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -2092,7 +2300,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
@@ -2124,7 +2332,7 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
@@ -2152,7 +2360,7 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -2184,7 +2392,7 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
@@ -2216,7 +2424,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -2248,7 +2456,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -2280,7 +2488,7 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>57</v>
       </c>
@@ -2312,7 +2520,7 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -2344,7 +2552,7 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>57</v>
       </c>
@@ -2376,7 +2584,7 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -2408,7 +2616,7 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -2440,7 +2648,7 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -2472,7 +2680,7 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -2504,7 +2712,7 @@
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
@@ -2536,7 +2744,7 @@
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>57</v>
       </c>
@@ -2568,7 +2776,7 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -2600,7 +2808,7 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>57</v>
       </c>
@@ -2628,7 +2836,7 @@
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -2660,7 +2868,7 @@
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
@@ -2692,7 +2900,7 @@
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -2724,7 +2932,7 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -2756,7 +2964,7 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -2788,7 +2996,7 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
     </row>
-    <row r="61" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -2820,7 +3028,7 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
     </row>
-    <row r="62" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
@@ -2852,7 +3060,7 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
     </row>
-    <row r="63" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>57</v>
       </c>
@@ -2884,7 +3092,7 @@
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
     </row>
-    <row r="64" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>57</v>
       </c>
@@ -2916,7 +3124,7 @@
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
     </row>
-    <row r="65" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>57</v>
       </c>
@@ -2948,7 +3156,7 @@
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
     </row>
-    <row r="66" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
@@ -2980,7 +3188,7 @@
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
     </row>
-    <row r="67" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>57</v>
       </c>
@@ -3012,7 +3220,7 @@
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
     </row>
-    <row r="68" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:20" ht="29" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>57</v>
       </c>
@@ -3040,7 +3248,7 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
     </row>
-    <row r="69" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:20" ht="29" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>57</v>
       </c>
@@ -3068,7 +3276,7 @@
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
     </row>
-    <row r="70" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>57</v>
       </c>
@@ -3100,7 +3308,7 @@
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
     </row>
-    <row r="71" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>57</v>
       </c>
@@ -3128,7 +3336,7 @@
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
     </row>
-    <row r="72" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>57</v>
       </c>
@@ -3160,7 +3368,7 @@
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
     </row>
-    <row r="73" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
@@ -3188,7 +3396,7 @@
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
     </row>
-    <row r="74" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -3220,7 +3428,7 @@
       <c r="S74" s="3"/>
       <c r="T74" s="3"/>
     </row>
-    <row r="75" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -3252,7 +3460,7 @@
       <c r="S75" s="3"/>
       <c r="T75" s="3"/>
     </row>
-    <row r="76" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>57</v>
       </c>
@@ -3284,7 +3492,7 @@
       <c r="S76" s="3"/>
       <c r="T76" s="3"/>
     </row>
-    <row r="77" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>57</v>
       </c>
@@ -3316,7 +3524,7 @@
       <c r="S77" s="3"/>
       <c r="T77" s="3"/>
     </row>
-    <row r="78" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>57</v>
       </c>
@@ -3348,7 +3556,7 @@
       <c r="S78" s="3"/>
       <c r="T78" s="3"/>
     </row>
-    <row r="79" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>57</v>
       </c>
@@ -3380,7 +3588,7 @@
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
     </row>
-    <row r="80" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
         <v>57</v>
       </c>
@@ -3408,7 +3616,7 @@
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
     </row>
-    <row r="81" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -3436,7 +3644,7 @@
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
     </row>
-    <row r="82" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
         <v>57</v>
       </c>
@@ -3464,7 +3672,7 @@
       <c r="S82" s="3"/>
       <c r="T82" s="3"/>
     </row>
-    <row r="83" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>57</v>
       </c>
@@ -3496,7 +3704,7 @@
       <c r="S83" s="3"/>
       <c r="T83" s="3"/>
     </row>
-    <row r="84" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>57</v>
       </c>
@@ -3528,7 +3736,7 @@
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
     </row>
-    <row r="85" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>57</v>
       </c>
@@ -3560,7 +3768,7 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
     </row>
-    <row r="86" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
         <v>57</v>
       </c>
@@ -3588,7 +3796,7 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>57</v>
       </c>
@@ -3620,7 +3828,7 @@
       <c r="S87" s="3"/>
       <c r="T87" s="3"/>
     </row>
-    <row r="88" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
         <v>57</v>
       </c>
@@ -3648,7 +3856,7 @@
       <c r="S88" s="3"/>
       <c r="T88" s="3"/>
     </row>
-    <row r="89" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
         <v>57</v>
       </c>
@@ -3676,7 +3884,7 @@
       <c r="S89" s="3"/>
       <c r="T89" s="3"/>
     </row>
-    <row r="90" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
         <v>57</v>
       </c>
@@ -3704,7 +3912,7 @@
       <c r="S90" s="3"/>
       <c r="T90" s="3"/>
     </row>
-    <row r="91" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
         <v>57</v>
       </c>
@@ -3736,7 +3944,7 @@
       <c r="S91" s="3"/>
       <c r="T91" s="3"/>
     </row>
-    <row r="92" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
         <v>57</v>
       </c>
@@ -3768,7 +3976,7 @@
       <c r="S92" s="3"/>
       <c r="T92" s="3"/>
     </row>
-    <row r="93" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
         <v>57</v>
       </c>
@@ -3800,7 +4008,7 @@
       <c r="S93" s="3"/>
       <c r="T93" s="3"/>
     </row>
-    <row r="94" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
         <v>57</v>
       </c>
@@ -3832,7 +4040,7 @@
       <c r="S94" s="3"/>
       <c r="T94" s="3"/>
     </row>
-    <row r="95" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
         <v>57</v>
       </c>
@@ -3864,7 +4072,7 @@
       <c r="S95" s="3"/>
       <c r="T95" s="3"/>
     </row>
-    <row r="96" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:20" ht="28" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
         <v>57</v>
       </c>
@@ -3896,7 +4104,7 @@
       <c r="S96" s="3"/>
       <c r="T96" s="3"/>
     </row>
-    <row r="97" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
         <v>57</v>
       </c>
@@ -3924,7 +4132,7 @@
       <c r="S97" s="3"/>
       <c r="T97" s="3"/>
     </row>
-    <row r="98" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>57</v>
       </c>
@@ -3956,7 +4164,7 @@
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
     </row>
-    <row r="99" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>57</v>
       </c>
@@ -3988,7 +4196,7 @@
       <c r="S99" s="3"/>
       <c r="T99" s="3"/>
     </row>
-    <row r="100" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
         <v>57</v>
       </c>
@@ -4020,7 +4228,7 @@
       <c r="S100" s="3"/>
       <c r="T100" s="3"/>
     </row>
-    <row r="101" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
         <v>57</v>
       </c>
@@ -4052,7 +4260,7 @@
       <c r="S101" s="3"/>
       <c r="T101" s="3"/>
     </row>
-    <row r="102" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>57</v>
       </c>
@@ -4084,7 +4292,7 @@
       <c r="S102" s="3"/>
       <c r="T102" s="3"/>
     </row>
-    <row r="103" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
         <v>57</v>
       </c>
@@ -4112,7 +4320,7 @@
       <c r="S103" s="3"/>
       <c r="T103" s="3"/>
     </row>
-    <row r="104" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>57</v>
       </c>
@@ -4140,7 +4348,7 @@
       <c r="S104" s="3"/>
       <c r="T104" s="3"/>
     </row>
-    <row r="105" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>57</v>
       </c>
@@ -4168,37 +4376,29 @@
       <c r="S105" s="3"/>
       <c r="T105" s="3"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>149</v>
       </c>
@@ -4209,7 +4409,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>152</v>
       </c>
@@ -4217,7 +4417,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>154</v>
       </c>
@@ -4225,7 +4425,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>156</v>
       </c>
@@ -4233,7 +4433,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>152</v>
       </c>
@@ -4241,7 +4441,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>159</v>
       </c>
@@ -4249,7 +4449,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>156</v>
       </c>
@@ -4257,7 +4457,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>152</v>
       </c>
@@ -4265,7 +4465,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>163</v>
       </c>
@@ -4273,7 +4473,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>165</v>
       </c>
@@ -4281,7 +4481,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>167</v>
       </c>
@@ -4289,7 +4489,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
         <v>169</v>
       </c>
@@ -4297,50 +4497,50 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>156</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
         <v>152</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
         <v>156</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>174</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
         <v>176</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
         <v>178</v>
       </c>
@@ -4348,46 +4548,31 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.43"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>180</v>
       </c>
@@ -4405,7 +4590,7 @@
       </c>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -4422,7 +4607,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -4439,7 +4624,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
@@ -4456,7 +4641,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -4474,44 +4659,37 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="10" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.43"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33.5" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" style="10" customWidth="1"/>
+    <col min="13" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>190</v>
       </c>
@@ -4531,22 +4709,25 @@
         <v>193</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>195</v>
       </c>
@@ -4560,17 +4741,20 @@
         <v>184</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="G2" s="12" t="n">
+      <c r="G2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" s="12">
         <v>42940</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>195</v>
       </c>
@@ -4586,16 +4770,16 @@
       <c r="E3" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="12" t="n">
+      <c r="H3" s="12"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="12">
         <v>42940</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>195</v>
       </c>
@@ -4614,16 +4798,16 @@
       <c r="F4" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="8"/>
-      <c r="J4" s="12" t="n">
+      <c r="H4" s="12"/>
+      <c r="I4" s="8"/>
+      <c r="K4" s="12">
         <v>42940</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>195</v>
       </c>
@@ -4637,17 +4821,20 @@
         <v>184</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="G5" s="12" t="n">
+      <c r="G5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" s="12">
         <v>42950</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>195</v>
       </c>
@@ -4663,16 +4850,16 @@
       <c r="E6" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="12" t="n">
+      <c r="H6" s="12"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="12">
         <v>42950</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>195</v>
       </c>
@@ -4691,16 +4878,16 @@
       <c r="F7" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="8"/>
-      <c r="J7" s="12" t="n">
+      <c r="H7" s="12"/>
+      <c r="I7" s="8"/>
+      <c r="K7" s="12">
         <v>42950</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>195</v>
       </c>
@@ -4719,11 +4906,11 @@
       <c r="F8" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="J8" s="12" t="n">
+      <c r="K8" s="12">
         <v>43004</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>195</v>
       </c>
@@ -4736,14 +4923,17 @@
       <c r="D9" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="G9" s="12" t="n">
+      <c r="G9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H9" s="12">
         <v>43011</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="I9" s="13" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>195</v>
       </c>
@@ -4759,13 +4949,13 @@
       <c r="E10" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="12" t="n">
+      <c r="H10" s="12"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="12">
         <v>43011</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>195</v>
       </c>
@@ -4784,19 +4974,14 @@
       <c r="F11" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="8"/>
-      <c r="J11" s="12" t="n">
+      <c r="H11" s="12"/>
+      <c r="I11" s="8"/>
+      <c r="K11" s="12">
         <v>43011</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing the individual importer
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/projects/work/openchs/openchs-server/openchs-server-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA71371-0694-DA4C-9A88-5B65D6BCD0E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,15 @@
     <sheet name="Calculated Fields" sheetId="3" r:id="rId3"/>
     <sheet name="Sheets" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="208">
   <si>
     <t>Form Name</t>
   </si>
@@ -632,51 +638,42 @@
     <t>8</t>
   </si>
   <si>
-    <t>Adolescent</t>
-  </si>
-  <si>
-    <t>Annual</t>
-  </si>
-  <si>
-    <t>Amalzar_Prathmik_3-8</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Followup</t>
-  </si>
-  <si>
-    <t>Madhyamik_Follow up_26-9</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>ambos 3-10</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
-    <t>Amalzar Secondary</t>
-  </si>
-  <si>
-    <t>Amalzar Primary</t>
-  </si>
-  <si>
-    <t>Aambos</t>
+    <t>IndividualRelationship</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>ઝગડિયા, કન્યા આદર્શ</t>
+  </si>
+  <si>
+    <t>Individual UUID</t>
+  </si>
+  <si>
+    <t>IndividualAUUID</t>
+  </si>
+  <si>
+    <t>IndividualBUUID</t>
+  </si>
+  <si>
+    <t>RelationshipType</t>
+  </si>
+  <si>
+    <t>EnterDateTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -727,9 +724,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF6A8759"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF9876AA"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -758,7 +791,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -785,7 +818,15 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,6 +904,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1130,12 +1174,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F89" sqref="F89"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1149,7 +1193,7 @@
     <col min="7" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1168,7 +1212,9 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="14" t="s">
+        <v>200</v>
+      </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -1183,22 +1229,23 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>203</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1214,7 +1261,7 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
     </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1226,7 +1273,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1245,7 +1292,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1257,10 +1304,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1276,7 +1323,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1288,14 +1335,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1311,7 +1354,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1323,10 +1366,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1342,7 +1389,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1354,14 +1401,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1377,22 +1420,25 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1409,7 +1455,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1418,13 +1464,13 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1441,7 +1487,7 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1450,10 +1496,14 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1469,7 +1519,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1478,7 +1528,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1497,7 +1547,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1506,14 +1556,10 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1529,7 +1575,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1538,13 +1584,13 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1561,7 +1607,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1570,13 +1616,13 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1593,7 +1639,7 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1602,13 +1648,13 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1625,22 +1671,23 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1656,23 +1703,22 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1688,19 +1734,23 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1716,7 +1766,7 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1725,7 +1775,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1744,7 +1794,7 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1753,7 +1803,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1772,7 +1822,7 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -1781,7 +1831,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1800,16 +1850,16 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1828,7 +1878,7 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
@@ -1837,14 +1887,10 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1860,7 +1906,7 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1869,10 +1915,14 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -1888,7 +1938,7 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>39</v>
       </c>
@@ -1897,7 +1947,7 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1916,7 +1966,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -1925,7 +1975,7 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1944,7 +1994,7 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
@@ -1953,7 +2003,7 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1972,7 +2022,7 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
@@ -1981,7 +2031,7 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2000,7 +2050,7 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -2009,7 +2059,7 @@
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2028,7 +2078,7 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20" ht="45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -2037,14 +2087,10 @@
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2060,7 +2106,7 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20" ht="45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2069,13 +2115,13 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2092,7 +2138,7 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -2101,10 +2147,14 @@
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -2120,16 +2170,16 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2148,23 +2198,19 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2180,7 +2226,7 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -2189,10 +2235,14 @@
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -2208,7 +2258,7 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
@@ -2217,14 +2267,10 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -2240,7 +2286,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -2249,13 +2295,13 @@
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -2272,7 +2318,7 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -2281,10 +2327,14 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2300,7 +2350,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
@@ -2309,14 +2359,10 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -2332,7 +2378,7 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
@@ -2341,10 +2387,14 @@
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -2360,7 +2410,7 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -2369,14 +2419,10 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -2392,7 +2438,7 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
@@ -2401,13 +2447,13 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -2424,7 +2470,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -2433,13 +2479,13 @@
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -2456,7 +2502,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -2465,13 +2511,13 @@
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -2488,7 +2534,7 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>57</v>
       </c>
@@ -2497,13 +2543,13 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -2520,7 +2566,7 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -2529,13 +2575,13 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -2552,7 +2598,7 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="47" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>57</v>
       </c>
@@ -2561,13 +2607,13 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -2584,7 +2630,7 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -2593,13 +2639,13 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -2616,7 +2662,7 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -2625,13 +2671,13 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -2648,7 +2694,7 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -2657,13 +2703,13 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -2680,7 +2726,7 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
     </row>
-    <row r="51" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -2689,13 +2735,13 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -2712,7 +2758,7 @@
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
     </row>
-    <row r="52" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
@@ -2721,13 +2767,13 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -2744,7 +2790,7 @@
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
     </row>
-    <row r="53" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>57</v>
       </c>
@@ -2753,13 +2799,13 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -2776,7 +2822,7 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -2785,13 +2831,13 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -2808,7 +2854,7 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>57</v>
       </c>
@@ -2817,10 +2863,14 @@
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -2836,7 +2886,7 @@
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
     </row>
-    <row r="56" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -2845,14 +2895,10 @@
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>83</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -2868,7 +2914,7 @@
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
     </row>
-    <row r="57" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
@@ -2877,13 +2923,13 @@
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -2900,7 +2946,7 @@
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
     </row>
-    <row r="58" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -2909,13 +2955,13 @@
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -2932,7 +2978,7 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" spans="1:20" ht="45" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -2941,13 +2987,13 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -2964,7 +3010,7 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
     </row>
-    <row r="60" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -2973,13 +3019,13 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -2996,7 +3042,7 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
     </row>
-    <row r="61" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -3005,13 +3051,13 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -3028,7 +3074,7 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
     </row>
-    <row r="62" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
@@ -3037,13 +3083,13 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -3060,7 +3106,7 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
     </row>
-    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>57</v>
       </c>
@@ -3069,13 +3115,13 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -3092,7 +3138,7 @@
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
     </row>
-    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>57</v>
       </c>
@@ -3101,13 +3147,13 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -3124,7 +3170,7 @@
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
     </row>
-    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>57</v>
       </c>
@@ -3133,13 +3179,13 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -3156,7 +3202,7 @@
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
     </row>
-    <row r="66" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
@@ -3165,13 +3211,13 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -3188,7 +3234,7 @@
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
     </row>
-    <row r="67" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>57</v>
       </c>
@@ -3197,13 +3243,13 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -3220,7 +3266,7 @@
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
     </row>
-    <row r="68" spans="1:20" ht="29" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>57</v>
       </c>
@@ -3229,10 +3275,14 @@
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -3248,7 +3298,7 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
     </row>
-    <row r="69" spans="1:20" ht="29" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" ht="31" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>57</v>
       </c>
@@ -3257,7 +3307,7 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -3276,7 +3326,7 @@
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
     </row>
-    <row r="70" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" ht="31" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>57</v>
       </c>
@@ -3285,14 +3335,10 @@
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>101</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -3308,7 +3354,7 @@
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
     </row>
-    <row r="71" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>57</v>
       </c>
@@ -3317,10 +3363,14 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -3336,7 +3386,7 @@
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
     </row>
-    <row r="72" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>57</v>
       </c>
@@ -3345,14 +3395,10 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>103</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -3368,7 +3414,7 @@
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
     </row>
-    <row r="73" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
@@ -3377,10 +3423,14 @@
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -3396,7 +3446,7 @@
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
     </row>
-    <row r="74" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -3405,14 +3455,10 @@
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>105</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -3428,7 +3474,7 @@
       <c r="S74" s="3"/>
       <c r="T74" s="3"/>
     </row>
-    <row r="75" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -3437,13 +3483,13 @@
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
@@ -3460,7 +3506,7 @@
       <c r="S75" s="3"/>
       <c r="T75" s="3"/>
     </row>
-    <row r="76" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>57</v>
       </c>
@@ -3469,13 +3515,13 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
@@ -3492,7 +3538,7 @@
       <c r="S76" s="3"/>
       <c r="T76" s="3"/>
     </row>
-    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>57</v>
       </c>
@@ -3501,13 +3547,13 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
@@ -3524,7 +3570,7 @@
       <c r="S77" s="3"/>
       <c r="T77" s="3"/>
     </row>
-    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>57</v>
       </c>
@@ -3533,13 +3579,13 @@
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
@@ -3556,7 +3602,7 @@
       <c r="S78" s="3"/>
       <c r="T78" s="3"/>
     </row>
-    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>57</v>
       </c>
@@ -3565,13 +3611,13 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
@@ -3588,7 +3634,7 @@
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
     </row>
-    <row r="80" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>57</v>
       </c>
@@ -3597,10 +3643,14 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -3616,7 +3666,7 @@
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
     </row>
-    <row r="81" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -3625,7 +3675,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -3644,7 +3694,7 @@
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
     </row>
-    <row r="82" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
         <v>57</v>
       </c>
@@ -3653,7 +3703,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
@@ -3672,7 +3722,7 @@
       <c r="S82" s="3"/>
       <c r="T82" s="3"/>
     </row>
-    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
         <v>57</v>
       </c>
@@ -3681,14 +3731,10 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>118</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -3704,7 +3750,7 @@
       <c r="S83" s="3"/>
       <c r="T83" s="3"/>
     </row>
-    <row r="84" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>57</v>
       </c>
@@ -3713,13 +3759,13 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
@@ -3736,7 +3782,7 @@
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
     </row>
-    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>57</v>
       </c>
@@ -3745,13 +3791,13 @@
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -3768,7 +3814,7 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
     </row>
-    <row r="86" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>57</v>
       </c>
@@ -3777,10 +3823,14 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
@@ -3796,7 +3846,7 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" spans="1:20" ht="45" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A87" s="3" t="s">
         <v>57</v>
       </c>
@@ -3805,14 +3855,10 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>125</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3828,7 +3874,7 @@
       <c r="S87" s="3"/>
       <c r="T87" s="3"/>
     </row>
-    <row r="88" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>57</v>
       </c>
@@ -3837,10 +3883,14 @@
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3856,7 +3906,7 @@
       <c r="S88" s="3"/>
       <c r="T88" s="3"/>
     </row>
-    <row r="89" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
         <v>57</v>
       </c>
@@ -3865,7 +3915,7 @@
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
@@ -3884,7 +3934,7 @@
       <c r="S89" s="3"/>
       <c r="T89" s="3"/>
     </row>
-    <row r="90" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
         <v>57</v>
       </c>
@@ -3893,7 +3943,7 @@
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
@@ -3912,7 +3962,7 @@
       <c r="S90" s="3"/>
       <c r="T90" s="3"/>
     </row>
-    <row r="91" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
         <v>57</v>
       </c>
@@ -3921,14 +3971,10 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -3944,7 +3990,7 @@
       <c r="S91" s="3"/>
       <c r="T91" s="3"/>
     </row>
-    <row r="92" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
         <v>57</v>
       </c>
@@ -3953,13 +3999,13 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
@@ -3976,7 +4022,7 @@
       <c r="S92" s="3"/>
       <c r="T92" s="3"/>
     </row>
-    <row r="93" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
         <v>57</v>
       </c>
@@ -3985,13 +4031,13 @@
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
@@ -4008,7 +4054,7 @@
       <c r="S93" s="3"/>
       <c r="T93" s="3"/>
     </row>
-    <row r="94" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
         <v>57</v>
       </c>
@@ -4017,13 +4063,13 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
@@ -4040,7 +4086,7 @@
       <c r="S94" s="3"/>
       <c r="T94" s="3"/>
     </row>
-    <row r="95" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
         <v>57</v>
       </c>
@@ -4049,13 +4095,13 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
@@ -4072,7 +4118,7 @@
       <c r="S95" s="3"/>
       <c r="T95" s="3"/>
     </row>
-    <row r="96" spans="1:20" ht="28" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
         <v>57</v>
       </c>
@@ -4081,13 +4127,13 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
@@ -4104,7 +4150,7 @@
       <c r="S96" s="3"/>
       <c r="T96" s="3"/>
     </row>
-    <row r="97" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:20" ht="30" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
         <v>57</v>
       </c>
@@ -4113,10 +4159,14 @@
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -4132,7 +4182,7 @@
       <c r="S97" s="3"/>
       <c r="T97" s="3"/>
     </row>
-    <row r="98" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
         <v>57</v>
       </c>
@@ -4141,14 +4191,10 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E98" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>140</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -4164,7 +4210,7 @@
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
     </row>
-    <row r="99" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>57</v>
       </c>
@@ -4173,13 +4219,13 @@
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
@@ -4196,7 +4242,7 @@
       <c r="S99" s="3"/>
       <c r="T99" s="3"/>
     </row>
-    <row r="100" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>57</v>
       </c>
@@ -4205,13 +4251,13 @@
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
@@ -4228,7 +4274,7 @@
       <c r="S100" s="3"/>
       <c r="T100" s="3"/>
     </row>
-    <row r="101" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:20" ht="30" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
         <v>57</v>
       </c>
@@ -4237,13 +4283,13 @@
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
@@ -4260,7 +4306,7 @@
       <c r="S101" s="3"/>
       <c r="T101" s="3"/>
     </row>
-    <row r="102" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>57</v>
       </c>
@@ -4269,13 +4315,13 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
@@ -4292,7 +4338,7 @@
       <c r="S102" s="3"/>
       <c r="T102" s="3"/>
     </row>
-    <row r="103" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
         <v>57</v>
       </c>
@@ -4301,10 +4347,14 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -4320,7 +4370,7 @@
       <c r="S103" s="3"/>
       <c r="T103" s="3"/>
     </row>
-    <row r="104" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>57</v>
       </c>
@@ -4329,7 +4379,7 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
@@ -4348,7 +4398,7 @@
       <c r="S104" s="3"/>
       <c r="T104" s="3"/>
     </row>
-    <row r="105" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>57</v>
       </c>
@@ -4357,7 +4407,7 @@
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
@@ -4376,7 +4426,80 @@
       <c r="S105" s="3"/>
       <c r="T105" s="3"/>
     </row>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="106" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A106" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3"/>
+      <c r="P106" s="3"/>
+      <c r="Q106" s="3"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="3"/>
+      <c r="T106" s="3"/>
+    </row>
+    <row r="107" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A107" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D107" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E107" s="20"/>
+      <c r="F107" s="20"/>
+    </row>
+    <row r="108" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A108" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D108" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A109" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B109" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D109" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+      <c r="A110" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B110" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D110" s="20" t="s">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4384,7 +4507,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4555,7 +4678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4665,11 +4788,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4689,7 +4812,7 @@
     <col min="13" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>190</v>
       </c>
@@ -4709,7 +4832,7 @@
         <v>193</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>8</v>
@@ -4741,8 +4864,8 @@
         <v>184</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="G2" t="s">
-        <v>208</v>
+      <c r="G2" s="17" t="s">
+        <v>202</v>
       </c>
       <c r="H2" s="12">
         <v>42940</v>
@@ -4758,227 +4881,20 @@
       <c r="A3" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>199</v>
-      </c>
+      <c r="B3" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
       <c r="H3" s="12"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="12">
-        <v>42940</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="8"/>
-      <c r="K4" s="12">
-        <v>42940</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="G5" t="s">
-        <v>209</v>
-      </c>
-      <c r="H5" s="12">
-        <v>42950</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="12">
-        <v>42950</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="8"/>
-      <c r="K7" s="12">
-        <v>42950</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="K8" s="12">
-        <v>43004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="G9" t="s">
-        <v>210</v>
-      </c>
-      <c r="H9" s="12">
-        <v>43011</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="12">
-        <v>43011</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="8"/>
-      <c r="K11" s="12">
-        <v>43011</v>
-      </c>
+      <c r="K3" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Resetting the excel files
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/projects/work/openchs/openchs-server/openchs-server-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA71371-0694-DA4C-9A88-5B65D6BCD0E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -18,15 +17,10 @@
     <sheet name="Calculated Fields" sheetId="3" r:id="rId3"/>
     <sheet name="Sheets" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -39,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="211">
   <si>
     <t>Form Name</t>
   </si>
@@ -638,42 +632,51 @@
     <t>8</t>
   </si>
   <si>
+    <t>Adolescent</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>Amalzar_Prathmik_3-8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Followup</t>
+  </si>
+  <si>
+    <t>Madhyamik_Follow up_26-9</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>ambos 3-10</t>
+  </si>
+  <si>
     <t>Address</t>
   </si>
   <si>
-    <t>IndividualRelationship</t>
-  </si>
-  <si>
-    <t>relationship</t>
-  </si>
-  <si>
-    <t>ઝગડિયા, કન્યા આદર્શ</t>
-  </si>
-  <si>
-    <t>Individual UUID</t>
-  </si>
-  <si>
-    <t>IndividualAUUID</t>
-  </si>
-  <si>
-    <t>IndividualBUUID</t>
-  </si>
-  <si>
-    <t>RelationshipType</t>
-  </si>
-  <si>
-    <t>EnterDateTime</t>
+    <t>Amalzar Secondary</t>
+  </si>
+  <si>
+    <t>Amalzar Primary</t>
+  </si>
+  <si>
+    <t>Aambos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -724,45 +727,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color rgb="FF9876AA"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -791,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -818,15 +785,7 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,9 +863,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1174,12 +1130,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1193,7 +1149,7 @@
     <col min="7" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1212,9 +1168,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>200</v>
-      </c>
+      <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -1229,23 +1183,22 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>203</v>
-      </c>
+      <c r="C2" s="3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1261,7 +1214,7 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
     </row>
-    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1292,7 +1245,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1304,10 +1257,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1323,7 +1276,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1335,10 +1288,14 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1354,7 +1311,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1366,14 +1323,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1389,7 +1342,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1401,10 +1354,14 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1420,25 +1377,22 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1455,7 +1409,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1464,13 +1418,13 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1487,7 +1441,7 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1496,14 +1450,10 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1519,7 +1469,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1528,7 +1478,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1547,7 +1497,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1556,10 +1506,14 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1575,7 +1529,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1584,13 +1538,13 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1607,7 +1561,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1616,13 +1570,13 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1639,7 +1593,7 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1648,13 +1602,13 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1671,23 +1625,22 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="D16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1703,22 +1656,23 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1734,23 +1688,19 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1766,7 +1716,7 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1775,7 +1725,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1794,7 +1744,7 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1803,7 +1753,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1822,7 +1772,7 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -1831,7 +1781,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1850,16 +1800,16 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1878,7 +1828,7 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
@@ -1887,10 +1837,14 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1906,7 +1860,7 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1915,14 +1869,10 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -1938,7 +1888,7 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>39</v>
       </c>
@@ -1947,7 +1897,7 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1966,7 +1916,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -1975,7 +1925,7 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -1994,7 +1944,7 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
@@ -2003,7 +1953,7 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2022,7 +1972,7 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
@@ -2031,7 +1981,7 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2050,7 +2000,7 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -2059,7 +2009,7 @@
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2078,7 +2028,7 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -2087,10 +2037,14 @@
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2106,7 +2060,7 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2115,13 +2069,13 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2138,7 +2092,7 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -2147,14 +2101,10 @@
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -2170,16 +2120,16 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2198,19 +2148,23 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2226,7 +2180,7 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -2235,14 +2189,10 @@
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -2258,7 +2208,7 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
@@ -2267,10 +2217,14 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -2286,7 +2240,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -2295,13 +2249,13 @@
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -2318,7 +2272,7 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -2327,14 +2281,10 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2350,7 +2300,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
@@ -2359,10 +2309,14 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -2378,7 +2332,7 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
@@ -2387,14 +2341,10 @@
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -2410,7 +2360,7 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -2419,10 +2369,14 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -2438,7 +2392,7 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
@@ -2447,13 +2401,13 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -2470,7 +2424,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -2479,13 +2433,13 @@
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -2502,7 +2456,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -2511,13 +2465,13 @@
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -2534,7 +2488,7 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>57</v>
       </c>
@@ -2543,13 +2497,13 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -2566,7 +2520,7 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -2575,13 +2529,13 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -2598,7 +2552,7 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="47" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>57</v>
       </c>
@@ -2607,13 +2561,13 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -2630,7 +2584,7 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -2639,13 +2593,13 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -2662,7 +2616,7 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -2671,13 +2625,13 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -2694,7 +2648,7 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -2703,13 +2657,13 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -2726,7 +2680,7 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
     </row>
-    <row r="51" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -2735,13 +2689,13 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -2758,7 +2712,7 @@
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
     </row>
-    <row r="52" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
@@ -2767,13 +2721,13 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -2790,7 +2744,7 @@
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
     </row>
-    <row r="53" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>57</v>
       </c>
@@ -2799,13 +2753,13 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -2822,7 +2776,7 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -2831,13 +2785,13 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -2854,7 +2808,7 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>57</v>
       </c>
@@ -2863,14 +2817,10 @@
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>81</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -2886,7 +2836,7 @@
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
     </row>
-    <row r="56" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -2895,10 +2845,14 @@
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -2914,7 +2868,7 @@
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
     </row>
-    <row r="57" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
@@ -2923,13 +2877,13 @@
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -2946,7 +2900,7 @@
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
     </row>
-    <row r="58" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -2955,13 +2909,13 @@
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -2978,7 +2932,7 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -2987,13 +2941,13 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -3010,7 +2964,7 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
     </row>
-    <row r="60" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -3019,13 +2973,13 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -3042,7 +2996,7 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
     </row>
-    <row r="61" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -3051,13 +3005,13 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -3074,7 +3028,7 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
     </row>
-    <row r="62" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
@@ -3083,13 +3037,13 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -3106,7 +3060,7 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
     </row>
-    <row r="63" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>57</v>
       </c>
@@ -3115,13 +3069,13 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -3138,7 +3092,7 @@
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
     </row>
-    <row r="64" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>57</v>
       </c>
@@ -3147,13 +3101,13 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -3170,7 +3124,7 @@
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
     </row>
-    <row r="65" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>57</v>
       </c>
@@ -3179,13 +3133,13 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -3202,7 +3156,7 @@
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
     </row>
-    <row r="66" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
@@ -3211,13 +3165,13 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -3234,7 +3188,7 @@
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
     </row>
-    <row r="67" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>57</v>
       </c>
@@ -3243,13 +3197,13 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -3266,7 +3220,7 @@
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
     </row>
-    <row r="68" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" ht="29" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>57</v>
       </c>
@@ -3275,14 +3229,10 @@
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>98</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -3298,7 +3248,7 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
     </row>
-    <row r="69" spans="1:20" ht="31" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" ht="29" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>57</v>
       </c>
@@ -3307,7 +3257,7 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -3326,7 +3276,7 @@
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
     </row>
-    <row r="70" spans="1:20" ht="31" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>57</v>
       </c>
@@ -3335,10 +3285,14 @@
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -3354,7 +3308,7 @@
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
     </row>
-    <row r="71" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>57</v>
       </c>
@@ -3363,14 +3317,10 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>101</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -3386,7 +3336,7 @@
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
     </row>
-    <row r="72" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>57</v>
       </c>
@@ -3395,10 +3345,14 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -3414,7 +3368,7 @@
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
     </row>
-    <row r="73" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
@@ -3423,14 +3377,10 @@
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>103</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -3446,7 +3396,7 @@
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
     </row>
-    <row r="74" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -3455,10 +3405,14 @@
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -3474,7 +3428,7 @@
       <c r="S74" s="3"/>
       <c r="T74" s="3"/>
     </row>
-    <row r="75" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -3483,13 +3437,13 @@
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
@@ -3506,7 +3460,7 @@
       <c r="S75" s="3"/>
       <c r="T75" s="3"/>
     </row>
-    <row r="76" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>57</v>
       </c>
@@ -3515,13 +3469,13 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
@@ -3538,7 +3492,7 @@
       <c r="S76" s="3"/>
       <c r="T76" s="3"/>
     </row>
-    <row r="77" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>57</v>
       </c>
@@ -3547,13 +3501,13 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
@@ -3570,7 +3524,7 @@
       <c r="S77" s="3"/>
       <c r="T77" s="3"/>
     </row>
-    <row r="78" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>57</v>
       </c>
@@ -3579,13 +3533,13 @@
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
@@ -3602,7 +3556,7 @@
       <c r="S78" s="3"/>
       <c r="T78" s="3"/>
     </row>
-    <row r="79" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>57</v>
       </c>
@@ -3611,13 +3565,13 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
@@ -3634,7 +3588,7 @@
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
     </row>
-    <row r="80" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
         <v>57</v>
       </c>
@@ -3643,14 +3597,10 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>113</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -3666,7 +3616,7 @@
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
     </row>
-    <row r="81" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -3675,7 +3625,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -3694,7 +3644,7 @@
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
     </row>
-    <row r="82" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
         <v>57</v>
       </c>
@@ -3703,7 +3653,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
@@ -3722,7 +3672,7 @@
       <c r="S82" s="3"/>
       <c r="T82" s="3"/>
     </row>
-    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>57</v>
       </c>
@@ -3731,10 +3681,14 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -3750,7 +3704,7 @@
       <c r="S83" s="3"/>
       <c r="T83" s="3"/>
     </row>
-    <row r="84" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>57</v>
       </c>
@@ -3759,13 +3713,13 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
@@ -3782,7 +3736,7 @@
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
     </row>
-    <row r="85" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>57</v>
       </c>
@@ -3791,13 +3745,13 @@
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -3814,7 +3768,7 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
     </row>
-    <row r="86" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
         <v>57</v>
       </c>
@@ -3823,14 +3777,10 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>122</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
@@ -3846,7 +3796,7 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:20" ht="45" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>57</v>
       </c>
@@ -3855,10 +3805,14 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3874,7 +3828,7 @@
       <c r="S87" s="3"/>
       <c r="T87" s="3"/>
     </row>
-    <row r="88" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
         <v>57</v>
       </c>
@@ -3883,14 +3837,10 @@
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>125</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3906,7 +3856,7 @@
       <c r="S88" s="3"/>
       <c r="T88" s="3"/>
     </row>
-    <row r="89" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
         <v>57</v>
       </c>
@@ -3915,7 +3865,7 @@
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
@@ -3934,7 +3884,7 @@
       <c r="S89" s="3"/>
       <c r="T89" s="3"/>
     </row>
-    <row r="90" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
         <v>57</v>
       </c>
@@ -3943,7 +3893,7 @@
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
@@ -3962,7 +3912,7 @@
       <c r="S90" s="3"/>
       <c r="T90" s="3"/>
     </row>
-    <row r="91" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
         <v>57</v>
       </c>
@@ -3971,10 +3921,14 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -3990,7 +3944,7 @@
       <c r="S91" s="3"/>
       <c r="T91" s="3"/>
     </row>
-    <row r="92" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
         <v>57</v>
       </c>
@@ -3999,13 +3953,13 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>47</v>
+        <v>129</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
@@ -4022,7 +3976,7 @@
       <c r="S92" s="3"/>
       <c r="T92" s="3"/>
     </row>
-    <row r="93" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
         <v>57</v>
       </c>
@@ -4031,13 +3985,13 @@
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
@@ -4054,7 +4008,7 @@
       <c r="S93" s="3"/>
       <c r="T93" s="3"/>
     </row>
-    <row r="94" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
         <v>57</v>
       </c>
@@ -4063,13 +4017,13 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
@@ -4086,7 +4040,7 @@
       <c r="S94" s="3"/>
       <c r="T94" s="3"/>
     </row>
-    <row r="95" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
         <v>57</v>
       </c>
@@ -4095,13 +4049,13 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
@@ -4118,7 +4072,7 @@
       <c r="S95" s="3"/>
       <c r="T95" s="3"/>
     </row>
-    <row r="96" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:20" ht="28" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
         <v>57</v>
       </c>
@@ -4127,13 +4081,13 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
@@ -4150,7 +4104,7 @@
       <c r="S96" s="3"/>
       <c r="T96" s="3"/>
     </row>
-    <row r="97" spans="1:20" ht="30" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
         <v>57</v>
       </c>
@@ -4159,14 +4113,10 @@
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>138</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -4182,7 +4132,7 @@
       <c r="S97" s="3"/>
       <c r="T97" s="3"/>
     </row>
-    <row r="98" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>57</v>
       </c>
@@ -4191,10 +4141,14 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
+        <v>140</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -4210,7 +4164,7 @@
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
     </row>
-    <row r="99" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>57</v>
       </c>
@@ -4219,13 +4173,13 @@
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
@@ -4242,7 +4196,7 @@
       <c r="S99" s="3"/>
       <c r="T99" s="3"/>
     </row>
-    <row r="100" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
         <v>57</v>
       </c>
@@ -4251,13 +4205,13 @@
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F100" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
@@ -4274,7 +4228,7 @@
       <c r="S100" s="3"/>
       <c r="T100" s="3"/>
     </row>
-    <row r="101" spans="1:20" ht="30" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
         <v>57</v>
       </c>
@@ -4283,13 +4237,13 @@
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
@@ -4306,7 +4260,7 @@
       <c r="S101" s="3"/>
       <c r="T101" s="3"/>
     </row>
-    <row r="102" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>57</v>
       </c>
@@ -4315,13 +4269,13 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
@@ -4338,7 +4292,7 @@
       <c r="S102" s="3"/>
       <c r="T102" s="3"/>
     </row>
-    <row r="103" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
         <v>57</v>
       </c>
@@ -4347,14 +4301,10 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>145</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -4370,7 +4320,7 @@
       <c r="S103" s="3"/>
       <c r="T103" s="3"/>
     </row>
-    <row r="104" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>57</v>
       </c>
@@ -4379,7 +4329,7 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
@@ -4398,7 +4348,7 @@
       <c r="S104" s="3"/>
       <c r="T104" s="3"/>
     </row>
-    <row r="105" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>57</v>
       </c>
@@ -4407,7 +4357,7 @@
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
@@ -4426,80 +4376,7 @@
       <c r="S105" s="3"/>
       <c r="T105" s="3"/>
     </row>
-    <row r="106" spans="1:20" ht="15" x14ac:dyDescent="0.15">
-      <c r="A106" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E106" s="3"/>
-      <c r="F106" s="3"/>
-      <c r="G106" s="3"/>
-      <c r="H106" s="3"/>
-      <c r="I106" s="3"/>
-      <c r="J106" s="3"/>
-      <c r="K106" s="3"/>
-      <c r="L106" s="3"/>
-      <c r="M106" s="3"/>
-      <c r="N106" s="3"/>
-      <c r="O106" s="3"/>
-      <c r="P106" s="3"/>
-      <c r="Q106" s="3"/>
-      <c r="R106" s="3"/>
-      <c r="S106" s="3"/>
-      <c r="T106" s="3"/>
-    </row>
-    <row r="107" spans="1:20" ht="15" x14ac:dyDescent="0.2">
-      <c r="A107" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="B107" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="D107" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-    </row>
-    <row r="108" spans="1:20" ht="15" x14ac:dyDescent="0.2">
-      <c r="A108" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="B108" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="D108" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="109" spans="1:20" ht="15" x14ac:dyDescent="0.2">
-      <c r="A109" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="B109" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="D109" s="20" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="110" spans="1:20" ht="15" x14ac:dyDescent="0.2">
-      <c r="A110" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="B110" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="D110" s="20" t="s">
-        <v>207</v>
-      </c>
-    </row>
+    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4507,7 +4384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4678,7 +4555,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4788,11 +4665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4812,7 +4689,7 @@
     <col min="13" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>190</v>
       </c>
@@ -4832,7 +4709,7 @@
         <v>193</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>8</v>
@@ -4864,8 +4741,8 @@
         <v>184</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="G2" s="17" t="s">
-        <v>202</v>
+      <c r="G2" t="s">
+        <v>208</v>
       </c>
       <c r="H2" s="12">
         <v>42940</v>
@@ -4881,20 +4758,227 @@
       <c r="A3" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>199</v>
+      </c>
       <c r="H3" s="12"/>
       <c r="I3" s="8"/>
-      <c r="K3" s="12"/>
+      <c r="J3" s="12">
+        <v>42940</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="8"/>
+      <c r="K4" s="12">
+        <v>42940</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="G5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" s="12">
+        <v>42950</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="12">
+        <v>42950</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="8"/>
+      <c r="K7" s="12">
+        <v>42950</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="K8" s="12">
+        <v>43004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H9" s="12">
+        <v>43011</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="12">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="8"/>
+      <c r="K11" s="12">
+        <v>43011</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Adding examples of relationship linking for individuals to the test import data
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/projects/work/openchs/openchs-server/openchs-server-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1400E4-DC19-3A45-A620-3D1863E0314B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,15 @@
     <sheet name="Calculated Fields" sheetId="3" r:id="rId3"/>
     <sheet name="Sheets" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="216">
   <si>
     <t>Form Name</t>
   </si>
@@ -666,12 +672,27 @@
   </si>
   <si>
     <t>Aambos</t>
+  </si>
+  <si>
+    <t>IndividualRelationship</t>
+  </si>
+  <si>
+    <t>IndividualAUUID</t>
+  </si>
+  <si>
+    <t>IndividualBUUID</t>
+  </si>
+  <si>
+    <t>EnterDateTime</t>
+  </si>
+  <si>
+    <t>RelationshipType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
@@ -863,6 +884,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1130,12 +1154,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1149,7 +1173,7 @@
     <col min="7" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1168,7 +1192,9 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -1183,7 +1209,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +1240,7 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
     </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1245,7 +1271,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1276,7 +1302,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1311,7 +1337,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1342,7 +1368,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1377,7 +1403,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1409,7 +1435,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1441,7 +1467,7 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1469,7 +1495,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1497,7 +1523,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -1529,7 +1555,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1561,7 +1587,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -1593,7 +1619,7 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -1625,7 +1651,7 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1656,7 +1682,7 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1688,7 +1714,7 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -1716,7 +1742,7 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1744,7 +1770,7 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1772,7 +1798,7 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -1800,7 +1826,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
@@ -1828,7 +1854,7 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
@@ -1860,7 +1886,7 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
@@ -1888,7 +1914,7 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>39</v>
       </c>
@@ -1916,7 +1942,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
@@ -1944,7 +1970,7 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
@@ -1972,7 +1998,7 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
@@ -2000,7 +2026,7 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>39</v>
       </c>
@@ -2028,7 +2054,7 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20" ht="45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -2060,7 +2086,7 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20" ht="45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2092,7 +2118,7 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
@@ -2120,7 +2146,7 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
@@ -2148,7 +2174,7 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>57</v>
       </c>
@@ -2180,7 +2206,7 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -2208,7 +2234,7 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>57</v>
       </c>
@@ -2240,7 +2266,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -2272,7 +2298,7 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -2300,7 +2326,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
@@ -2332,7 +2358,7 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
@@ -2360,7 +2386,7 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -2392,7 +2418,7 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
@@ -2424,7 +2450,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>57</v>
       </c>
@@ -2456,7 +2482,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -2488,7 +2514,7 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>57</v>
       </c>
@@ -2520,7 +2546,7 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -2552,7 +2578,7 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="47" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>57</v>
       </c>
@@ -2584,7 +2610,7 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
@@ -2616,7 +2642,7 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -2648,7 +2674,7 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -2680,7 +2706,7 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
     </row>
-    <row r="51" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>57</v>
       </c>
@@ -2712,7 +2738,7 @@
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
     </row>
-    <row r="52" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
@@ -2744,7 +2770,7 @@
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
     </row>
-    <row r="53" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>57</v>
       </c>
@@ -2776,7 +2802,7 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -2808,7 +2834,7 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
         <v>57</v>
       </c>
@@ -2836,7 +2862,7 @@
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
     </row>
-    <row r="56" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>57</v>
       </c>
@@ -2868,7 +2894,7 @@
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
     </row>
-    <row r="57" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
@@ -2900,7 +2926,7 @@
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
     </row>
-    <row r="58" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -2932,7 +2958,7 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" spans="1:20" ht="45" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -2964,7 +2990,7 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
     </row>
-    <row r="60" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -2996,7 +3022,7 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
     </row>
-    <row r="61" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -3028,7 +3054,7 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
     </row>
-    <row r="62" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
@@ -3060,7 +3086,7 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
     </row>
-    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>57</v>
       </c>
@@ -3092,7 +3118,7 @@
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
     </row>
-    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>57</v>
       </c>
@@ -3124,7 +3150,7 @@
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
     </row>
-    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>57</v>
       </c>
@@ -3156,7 +3182,7 @@
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
     </row>
-    <row r="66" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
@@ -3188,7 +3214,7 @@
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
     </row>
-    <row r="67" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>57</v>
       </c>
@@ -3220,7 +3246,7 @@
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
     </row>
-    <row r="68" spans="1:20" ht="29" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" ht="31" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>57</v>
       </c>
@@ -3248,7 +3274,7 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
     </row>
-    <row r="69" spans="1:20" ht="29" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" ht="31" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>57</v>
       </c>
@@ -3308,7 +3334,7 @@
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
     </row>
-    <row r="71" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>57</v>
       </c>
@@ -3336,7 +3362,7 @@
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
     </row>
-    <row r="72" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>57</v>
       </c>
@@ -3368,7 +3394,7 @@
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
     </row>
-    <row r="73" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
@@ -3396,7 +3422,7 @@
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
     </row>
-    <row r="74" spans="1:20" ht="30" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -3428,7 +3454,7 @@
       <c r="S74" s="3"/>
       <c r="T74" s="3"/>
     </row>
-    <row r="75" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
@@ -3460,7 +3486,7 @@
       <c r="S75" s="3"/>
       <c r="T75" s="3"/>
     </row>
-    <row r="76" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>57</v>
       </c>
@@ -3492,7 +3518,7 @@
       <c r="S76" s="3"/>
       <c r="T76" s="3"/>
     </row>
-    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>57</v>
       </c>
@@ -3524,7 +3550,7 @@
       <c r="S77" s="3"/>
       <c r="T77" s="3"/>
     </row>
-    <row r="78" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>57</v>
       </c>
@@ -3556,7 +3582,7 @@
       <c r="S78" s="3"/>
       <c r="T78" s="3"/>
     </row>
-    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>57</v>
       </c>
@@ -3588,7 +3614,7 @@
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
     </row>
-    <row r="80" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
         <v>57</v>
       </c>
@@ -3616,7 +3642,7 @@
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
     </row>
-    <row r="81" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -3644,7 +3670,7 @@
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
     </row>
-    <row r="82" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
         <v>57</v>
       </c>
@@ -3672,7 +3698,7 @@
       <c r="S82" s="3"/>
       <c r="T82" s="3"/>
     </row>
-    <row r="83" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>57</v>
       </c>
@@ -3704,7 +3730,7 @@
       <c r="S83" s="3"/>
       <c r="T83" s="3"/>
     </row>
-    <row r="84" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>57</v>
       </c>
@@ -3736,7 +3762,7 @@
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
     </row>
-    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>57</v>
       </c>
@@ -3768,7 +3794,7 @@
       <c r="S85" s="3"/>
       <c r="T85" s="3"/>
     </row>
-    <row r="86" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A86" s="3" t="s">
         <v>57</v>
       </c>
@@ -3796,7 +3822,7 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" spans="1:20" ht="45" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>57</v>
       </c>
@@ -3828,7 +3854,7 @@
       <c r="S87" s="3"/>
       <c r="T87" s="3"/>
     </row>
-    <row r="88" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A88" s="3" t="s">
         <v>57</v>
       </c>
@@ -3856,7 +3882,7 @@
       <c r="S88" s="3"/>
       <c r="T88" s="3"/>
     </row>
-    <row r="89" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A89" s="3" t="s">
         <v>57</v>
       </c>
@@ -3884,7 +3910,7 @@
       <c r="S89" s="3"/>
       <c r="T89" s="3"/>
     </row>
-    <row r="90" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A90" s="3" t="s">
         <v>57</v>
       </c>
@@ -3912,7 +3938,7 @@
       <c r="S90" s="3"/>
       <c r="T90" s="3"/>
     </row>
-    <row r="91" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
         <v>57</v>
       </c>
@@ -3944,7 +3970,7 @@
       <c r="S91" s="3"/>
       <c r="T91" s="3"/>
     </row>
-    <row r="92" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A92" s="3" t="s">
         <v>57</v>
       </c>
@@ -3976,7 +4002,7 @@
       <c r="S92" s="3"/>
       <c r="T92" s="3"/>
     </row>
-    <row r="93" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A93" s="3" t="s">
         <v>57</v>
       </c>
@@ -4008,7 +4034,7 @@
       <c r="S93" s="3"/>
       <c r="T93" s="3"/>
     </row>
-    <row r="94" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A94" s="3" t="s">
         <v>57</v>
       </c>
@@ -4040,7 +4066,7 @@
       <c r="S94" s="3"/>
       <c r="T94" s="3"/>
     </row>
-    <row r="95" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
         <v>57</v>
       </c>
@@ -4072,7 +4098,7 @@
       <c r="S95" s="3"/>
       <c r="T95" s="3"/>
     </row>
-    <row r="96" spans="1:20" ht="28" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:20" ht="30" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
         <v>57</v>
       </c>
@@ -4104,7 +4130,7 @@
       <c r="S96" s="3"/>
       <c r="T96" s="3"/>
     </row>
-    <row r="97" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
         <v>57</v>
       </c>
@@ -4132,7 +4158,7 @@
       <c r="S97" s="3"/>
       <c r="T97" s="3"/>
     </row>
-    <row r="98" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>57</v>
       </c>
@@ -4164,7 +4190,7 @@
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
     </row>
-    <row r="99" spans="1:20" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>57</v>
       </c>
@@ -4196,7 +4222,7 @@
       <c r="S99" s="3"/>
       <c r="T99" s="3"/>
     </row>
-    <row r="100" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:20" ht="30" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
         <v>57</v>
       </c>
@@ -4228,7 +4254,7 @@
       <c r="S100" s="3"/>
       <c r="T100" s="3"/>
     </row>
-    <row r="101" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
         <v>57</v>
       </c>
@@ -4260,7 +4286,7 @@
       <c r="S101" s="3"/>
       <c r="T101" s="3"/>
     </row>
-    <row r="102" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>57</v>
       </c>
@@ -4292,7 +4318,7 @@
       <c r="S102" s="3"/>
       <c r="T102" s="3"/>
     </row>
-    <row r="103" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
         <v>57</v>
       </c>
@@ -4320,7 +4346,7 @@
       <c r="S103" s="3"/>
       <c r="T103" s="3"/>
     </row>
-    <row r="104" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>57</v>
       </c>
@@ -4348,7 +4374,7 @@
       <c r="S104" s="3"/>
       <c r="T104" s="3"/>
     </row>
-    <row r="105" spans="1:20" ht="14" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>57</v>
       </c>
@@ -4376,6 +4402,50 @@
       <c r="S105" s="3"/>
       <c r="T105" s="3"/>
     </row>
+    <row r="106" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A106" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A107" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A108" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A109" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -4384,7 +4454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4555,7 +4625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4665,10 +4735,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -4689,7 +4759,7 @@
     <col min="13" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
Adding the relationship sheet
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/projects/work/openchs/openchs-server/openchs-server-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1400E4-DC19-3A45-A620-3D1863E0314B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F231C4-A63E-034E-94E6-534BADE07ED6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="217">
   <si>
     <t>Form Name</t>
   </si>
@@ -687,6 +687,9 @@
   </si>
   <si>
     <t>RelationshipType</t>
+  </si>
+  <si>
+    <t>Relationship</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
     </sheetView>
@@ -4736,10 +4739,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5050,6 +5053,20 @@
         <v>43011</v>
       </c>
     </row>
+    <row r="12" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Minor reformatting and removing all the errors from the excel sheet
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/projects/work/openchs/openchs-server/openchs-server-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F231C4-A63E-034E-94E6-534BADE07ED6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FD2099-6B34-DF46-ACE9-E6410F0AD48E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Calculated Fields" sheetId="3" r:id="rId3"/>
     <sheet name="Sheets" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="218">
   <si>
     <t>Form Name</t>
   </si>
@@ -608,9 +608,6 @@
     <t>[a-zA-Z]+\s+([a-zA-Z]+).*</t>
   </si>
   <si>
-    <t>.*(\d).*</t>
-  </si>
-  <si>
     <t>File Name</t>
   </si>
   <si>
@@ -641,9 +638,6 @@
     <t>Adolescent</t>
   </si>
   <si>
-    <t>Annual</t>
-  </si>
-  <si>
     <t>Amalzar_Prathmik_3-8</t>
   </si>
   <si>
@@ -656,24 +650,12 @@
     <t>Madhyamik_Follow up_26-9</t>
   </si>
   <si>
-    <t>Monthly</t>
-  </si>
-  <si>
     <t>ambos 3-10</t>
   </si>
   <si>
     <t>Address</t>
   </si>
   <si>
-    <t>Amalzar Secondary</t>
-  </si>
-  <si>
-    <t>Amalzar Primary</t>
-  </si>
-  <si>
-    <t>Aambos</t>
-  </si>
-  <si>
     <t>IndividualRelationship</t>
   </si>
   <si>
@@ -690,6 +672,27 @@
   </si>
   <si>
     <t>Relationship</t>
+  </si>
+  <si>
+    <t>Individual UUID</t>
+  </si>
+  <si>
+    <t>Enrolment UUID</t>
+  </si>
+  <si>
+    <t>અમલઝર માધ્યમિક</t>
+  </si>
+  <si>
+    <t>અમલઝર પ્રાથમિક</t>
+  </si>
+  <si>
+    <t>આંબોસ</t>
+  </si>
+  <si>
+    <t>Annual Visit</t>
+  </si>
+  <si>
+    <t>Monthly Visit</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -755,6 +758,11 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -782,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -810,6 +818,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1158,11 +1167,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1048576"/>
+  <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1196,9 +1205,11 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="H1" s="3"/>
+        <v>205</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>201</v>
+      </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -1212,22 +1223,23 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+        <v>211</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>211</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1255,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1274,7 +1286,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1286,10 +1298,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1305,7 +1317,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1317,14 +1329,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1352,10 +1360,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1383,14 +1395,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1413,15 +1421,18 @@
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1447,13 +1458,13 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1479,10 +1490,14 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1507,7 +1522,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1535,14 +1550,10 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1567,13 +1578,13 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1599,13 +1610,13 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1631,13 +1642,13 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1656,20 +1667,21 @@
     </row>
     <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1685,7 +1697,7 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1694,13 +1706,13 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>32</v>
+        <v>211</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1717,19 +1729,23 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1747,14 +1763,17 @@
     </row>
     <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="D19" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1775,17 +1794,21 @@
     </row>
     <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1810,7 +1833,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1831,14 +1854,14 @@
     </row>
     <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1859,21 +1882,17 @@
     </row>
     <row r="23" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -1891,14 +1910,14 @@
     </row>
     <row r="24" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1926,7 +1945,7 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1954,10 +1973,14 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1982,7 +2005,7 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -2010,7 +2033,7 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2038,7 +2061,7 @@
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2057,7 +2080,7 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
@@ -2066,14 +2089,10 @@
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2089,7 +2108,7 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2098,14 +2117,10 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -2130,7 +2145,7 @@
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2149,19 +2164,23 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -2177,22 +2196,22 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -2209,19 +2228,19 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -2237,23 +2256,19 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -2269,7 +2284,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
@@ -2278,16 +2293,18 @@
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>64</v>
+        <v>212</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="H37" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2301,7 +2318,7 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
         <v>57</v>
       </c>
@@ -2310,10 +2327,14 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+        <v>58</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2329,7 +2350,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>57</v>
       </c>
@@ -2338,14 +2359,10 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -2370,10 +2387,14 @@
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -2389,7 +2410,7 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>57</v>
       </c>
@@ -2398,13 +2419,13 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -2421,7 +2442,7 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>57</v>
       </c>
@@ -2430,14 +2451,10 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -2462,13 +2479,13 @@
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -2485,7 +2502,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -2494,14 +2511,10 @@
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>71</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -2517,7 +2530,7 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>57</v>
       </c>
@@ -2526,13 +2539,13 @@
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -2558,13 +2571,13 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -2590,13 +2603,13 @@
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -2622,13 +2635,13 @@
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -2645,7 +2658,7 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>57</v>
       </c>
@@ -2654,13 +2667,13 @@
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -2677,7 +2690,7 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -2686,13 +2699,13 @@
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -2718,13 +2731,13 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -2750,13 +2763,13 @@
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -2782,13 +2795,13 @@
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -2805,7 +2818,7 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -2814,13 +2827,13 @@
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -2837,7 +2850,7 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>57</v>
       </c>
@@ -2846,10 +2859,14 @@
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -2874,13 +2891,13 @@
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -2906,13 +2923,13 @@
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -2938,13 +2955,13 @@
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -2961,7 +2978,7 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -2970,14 +2987,10 @@
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>86</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
@@ -2993,7 +3006,7 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
     </row>
-    <row r="60" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -3002,13 +3015,13 @@
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -3025,7 +3038,7 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
     </row>
-    <row r="61" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>57</v>
       </c>
@@ -3034,13 +3047,13 @@
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -3057,7 +3070,7 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
     </row>
-    <row r="62" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
@@ -3066,13 +3079,13 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -3089,7 +3102,7 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
     </row>
-    <row r="63" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>57</v>
       </c>
@@ -3098,13 +3111,13 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -3121,7 +3134,7 @@
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
     </row>
-    <row r="64" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>57</v>
       </c>
@@ -3130,13 +3143,13 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -3162,13 +3175,13 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -3185,7 +3198,7 @@
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
     </row>
-    <row r="66" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
@@ -3194,13 +3207,13 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -3226,13 +3239,13 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -3249,7 +3262,7 @@
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
     </row>
-    <row r="68" spans="1:20" ht="31" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>57</v>
       </c>
@@ -3258,10 +3271,14 @@
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -3277,7 +3294,7 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
     </row>
-    <row r="69" spans="1:20" ht="31" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>57</v>
       </c>
@@ -3286,10 +3303,14 @@
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -3305,7 +3326,7 @@
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
     </row>
-    <row r="70" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>57</v>
       </c>
@@ -3314,13 +3335,13 @@
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
@@ -3346,10 +3367,14 @@
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -3365,7 +3390,7 @@
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
     </row>
-    <row r="72" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" ht="31" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>57</v>
       </c>
@@ -3374,14 +3399,10 @@
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>103</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -3397,7 +3418,7 @@
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
     </row>
-    <row r="73" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:20" ht="31" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>57</v>
       </c>
@@ -3406,10 +3427,10 @@
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -3425,7 +3446,7 @@
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
     </row>
-    <row r="74" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -3434,13 +3455,13 @@
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
@@ -3466,14 +3487,10 @@
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>107</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
@@ -3498,13 +3515,13 @@
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
@@ -3521,7 +3538,7 @@
       <c r="S76" s="3"/>
       <c r="T76" s="3"/>
     </row>
-    <row r="77" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A77" s="3" t="s">
         <v>57</v>
       </c>
@@ -3530,14 +3547,10 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>110</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -3553,7 +3566,7 @@
       <c r="S77" s="3"/>
       <c r="T77" s="3"/>
     </row>
-    <row r="78" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>57</v>
       </c>
@@ -3562,13 +3575,13 @@
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
@@ -3594,13 +3607,13 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
@@ -3617,7 +3630,7 @@
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
     </row>
-    <row r="80" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>57</v>
       </c>
@@ -3626,10 +3639,14 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -3645,7 +3662,7 @@
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
     </row>
-    <row r="81" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>57</v>
       </c>
@@ -3654,10 +3671,14 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -3673,7 +3694,7 @@
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
     </row>
-    <row r="82" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>57</v>
       </c>
@@ -3682,10 +3703,14 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
+        <v>111</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
@@ -3710,13 +3735,13 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
@@ -3733,7 +3758,7 @@
       <c r="S83" s="3"/>
       <c r="T83" s="3"/>
     </row>
-    <row r="84" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A84" s="3" t="s">
         <v>57</v>
       </c>
@@ -3742,14 +3767,10 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>120</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -3765,7 +3786,7 @@
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
     </row>
-    <row r="85" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A85" s="3" t="s">
         <v>57</v>
       </c>
@@ -3774,14 +3795,10 @@
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>122</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
@@ -3806,7 +3823,7 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -3825,7 +3842,7 @@
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
     </row>
-    <row r="87" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>57</v>
       </c>
@@ -3834,13 +3851,13 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
@@ -3857,7 +3874,7 @@
       <c r="S87" s="3"/>
       <c r="T87" s="3"/>
     </row>
-    <row r="88" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>57</v>
       </c>
@@ -3866,10 +3883,14 @@
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3885,7 +3906,7 @@
       <c r="S88" s="3"/>
       <c r="T88" s="3"/>
     </row>
-    <row r="89" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>57</v>
       </c>
@@ -3894,10 +3915,14 @@
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -3922,7 +3947,7 @@
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
@@ -3941,7 +3966,7 @@
       <c r="S90" s="3"/>
       <c r="T90" s="3"/>
     </row>
-    <row r="91" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>57</v>
       </c>
@@ -3950,13 +3975,13 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
@@ -3982,14 +4007,10 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>130</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -4014,14 +4035,10 @@
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>132</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -4046,14 +4063,10 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>134</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -4078,13 +4091,13 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
@@ -4101,7 +4114,7 @@
       <c r="S95" s="3"/>
       <c r="T95" s="3"/>
     </row>
-    <row r="96" spans="1:20" ht="30" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A96" s="3" t="s">
         <v>57</v>
       </c>
@@ -4110,13 +4123,13 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
@@ -4142,10 +4155,14 @@
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
+        <v>131</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -4161,7 +4178,7 @@
       <c r="S97" s="3"/>
       <c r="T97" s="3"/>
     </row>
-    <row r="98" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
         <v>57</v>
       </c>
@@ -4170,13 +4187,13 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E98" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
@@ -4193,7 +4210,7 @@
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
     </row>
-    <row r="99" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
         <v>57</v>
       </c>
@@ -4202,13 +4219,13 @@
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E99" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>142</v>
+        <v>135</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
@@ -4234,13 +4251,13 @@
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
@@ -4266,14 +4283,10 @@
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>144</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
@@ -4289,7 +4302,7 @@
       <c r="S101" s="3"/>
       <c r="T101" s="3"/>
     </row>
-    <row r="102" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>57</v>
       </c>
@@ -4298,13 +4311,13 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
@@ -4321,7 +4334,7 @@
       <c r="S102" s="3"/>
       <c r="T102" s="3"/>
     </row>
-    <row r="103" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>57</v>
       </c>
@@ -4330,10 +4343,14 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -4349,7 +4366,7 @@
       <c r="S103" s="3"/>
       <c r="T103" s="3"/>
     </row>
-    <row r="104" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:20" ht="30" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>57</v>
       </c>
@@ -4358,10 +4375,14 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
+        <v>143</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
@@ -4386,10 +4407,14 @@
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
+        <v>144</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -4407,49 +4432,176 @@
     </row>
     <row r="106" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
-        <v>211</v>
+        <v>57</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>211</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>212</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3"/>
+      <c r="P106" s="3"/>
+      <c r="Q106" s="3"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="3"/>
+      <c r="T106" s="3"/>
     </row>
     <row r="107" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
-        <v>211</v>
+        <v>57</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>211</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C107" s="3"/>
       <c r="D107" s="3" t="s">
-        <v>213</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+      <c r="M107" s="3"/>
+      <c r="N107" s="3"/>
+      <c r="O107" s="3"/>
+      <c r="P107" s="3"/>
+      <c r="Q107" s="3"/>
+      <c r="R107" s="3"/>
+      <c r="S107" s="3"/>
+      <c r="T107" s="3"/>
     </row>
     <row r="108" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A108" s="3" t="s">
-        <v>211</v>
+        <v>57</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>211</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>214</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="3"/>
+      <c r="T108" s="3"/>
     </row>
     <row r="109" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A109" s="3" t="s">
-        <v>211</v>
+        <v>57</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>211</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C109" s="3"/>
       <c r="D109" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>148</v>
+      </c>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
+      <c r="O109" s="3"/>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="3"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="3"/>
+      <c r="T109" s="3"/>
+    </row>
+    <row r="110" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A110" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A111" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" ht="15" x14ac:dyDescent="0.15">
+      <c r="A112" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+      <c r="A113" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4629,10 +4781,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4693,7 +4845,7 @@
       <c r="D3" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="15" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4719,16 +4871,50 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>148</v>
+        <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>185</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -4741,8 +4927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4764,25 +4950,25 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>180</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>181</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>193</v>
-      </c>
       <c r="G1" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>8</v>
@@ -4794,7 +4980,7 @@
         <v>30</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>148</v>
@@ -4802,46 +4988,46 @@
     </row>
     <row r="2" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>184</v>
       </c>
       <c r="E2" s="8"/>
       <c r="G2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="H2" s="12">
         <v>42940</v>
       </c>
       <c r="I2" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="8"/>
@@ -4849,27 +5035,27 @@
         <v>42940</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="8"/>
@@ -4877,51 +5063,51 @@
         <v>42940</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>184</v>
       </c>
       <c r="E5" s="8"/>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="H5" s="12">
         <v>42950</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="8"/>
@@ -4929,27 +5115,27 @@
         <v>42950</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="8"/>
@@ -4957,27 +5143,27 @@
         <v>42950</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>205</v>
+        <v>198</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>217</v>
       </c>
       <c r="K8" s="12">
         <v>43004</v>
@@ -4985,42 +5171,42 @@
     </row>
     <row r="9" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>184</v>
       </c>
       <c r="G9" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="H9" s="12">
         <v>43011</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="8"/>
@@ -5030,22 +5216,22 @@
     </row>
     <row r="11" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="8"/>
@@ -5055,16 +5241,16 @@
     </row>
     <row r="12" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finishing off checklist importer, it runs in a synchronous mode
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/projects/work/openchs/openchs-server/openchs-server-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FD2099-6B34-DF46-ACE9-E6410F0AD48E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84820A3D-5B7B-0444-A23D-28121EF1B078}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="225">
   <si>
     <t>Form Name</t>
   </si>
@@ -693,6 +693,27 @@
   </si>
   <si>
     <t>Monthly Visit</t>
+  </si>
+  <si>
+    <t>Checklist</t>
+  </si>
+  <si>
+    <t>ChecklistItem</t>
+  </si>
+  <si>
+    <t>Completion Date</t>
+  </si>
+  <si>
+    <t>Vaccination</t>
+  </si>
+  <si>
+    <t>Checklist Name</t>
+  </si>
+  <si>
+    <t>Base Date</t>
+  </si>
+  <si>
+    <t>Item Name</t>
   </si>
 </sst>
 </file>
@@ -703,7 +724,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -714,54 +735,61 @@
       <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -790,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -819,6 +847,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1167,11 +1196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T113"/>
+  <dimension ref="A1:T117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1210,7 +1239,9 @@
       <c r="H1" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="I1" s="3" t="s">
+        <v>218</v>
+      </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -4588,7 +4619,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
         <v>205</v>
       </c>
@@ -4600,6 +4631,62 @@
       </c>
       <c r="G113" s="3" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A114" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="I114" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A115" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="I115" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A116" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="I116" s="16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A117" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D117" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="I117" s="16" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -4784,7 +4871,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4925,10 +5012,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4939,16 +5026,16 @@
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" style="10" customWidth="1"/>
-    <col min="13" max="1025" width="14.5" customWidth="1"/>
+    <col min="7" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" style="10" customWidth="1"/>
+    <col min="14" max="1026" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>189</v>
       </c>
@@ -4970,23 +5057,26 @@
       <c r="G1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>194</v>
       </c>
@@ -5003,17 +5093,17 @@
       <c r="G2" t="s">
         <v>213</v>
       </c>
-      <c r="H2" s="12">
+      <c r="I2" s="12">
         <v>42940</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>194</v>
       </c>
@@ -5029,16 +5119,16 @@
       <c r="E3" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="12">
+      <c r="I3" s="12"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="12">
         <v>42940</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>194</v>
       </c>
@@ -5057,16 +5147,16 @@
       <c r="F4" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="8"/>
-      <c r="K4" s="12">
+      <c r="I4" s="12"/>
+      <c r="J4" s="8"/>
+      <c r="L4" s="12">
         <v>42940</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>194</v>
       </c>
@@ -5083,17 +5173,17 @@
       <c r="G5" t="s">
         <v>214</v>
       </c>
-      <c r="H5" s="12">
+      <c r="I5" s="12">
         <v>42950</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>194</v>
       </c>
@@ -5109,16 +5199,16 @@
       <c r="E6" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="12">
+      <c r="I6" s="12"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="12">
         <v>42950</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="8" t="s">
         <v>194</v>
       </c>
@@ -5137,16 +5227,16 @@
       <c r="F7" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="8"/>
-      <c r="K7" s="12">
+      <c r="I7" s="12"/>
+      <c r="J7" s="8"/>
+      <c r="L7" s="12">
         <v>42950</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
         <v>194</v>
       </c>
@@ -5165,11 +5255,11 @@
       <c r="F8" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="K8" s="12">
+      <c r="L8" s="12">
         <v>43004</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>194</v>
       </c>
@@ -5185,14 +5275,14 @@
       <c r="G9" t="s">
         <v>215</v>
       </c>
-      <c r="H9" s="12">
+      <c r="I9" s="12">
         <v>43011</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>194</v>
       </c>
@@ -5208,13 +5298,13 @@
       <c r="E10" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="12">
+      <c r="I10" s="12"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="12">
         <v>43011</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>194</v>
       </c>
@@ -5233,13 +5323,13 @@
       <c r="F11" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="8"/>
-      <c r="K11" s="12">
+      <c r="I11" s="12"/>
+      <c r="J11" s="8"/>
+      <c r="L11" s="12">
         <v>43011</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="8" t="s">
         <v>194</v>
       </c>
@@ -5251,6 +5341,26 @@
       </c>
       <c r="D12" s="8" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed form name as a field, it was duplicate created by mistake
</commit_message>
<xml_diff>
--- a/openchs-server-api/src/test/resources/Import MetaData.xlsx
+++ b/openchs-server-api/src/test/resources/Import MetaData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="226">
-  <si>
-    <t xml:space="preserve">Form Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="225">
+  <si>
+    <t xml:space="preserve">User File Type</t>
   </si>
   <si>
     <t xml:space="preserve">Form Type</t>
@@ -602,9 +602,6 @@
   </si>
   <si>
     <t xml:space="preserve">Only Father alive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User File Type</t>
   </si>
   <si>
     <t xml:space="preserve">Entity Type</t>
@@ -982,10 +979,10 @@
   </sheetPr>
   <dimension ref="A1:T117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D114" activeCellId="0" sqref="D114"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -999,7 +996,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4687,19 +4684,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="F1" s="6"/>
     </row>
@@ -4708,16 +4705,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4725,16 +4722,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4742,16 +4739,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4759,16 +4756,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4776,16 +4773,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4793,16 +4790,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4823,8 +4820,8 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4846,31 +4843,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>12</v>
@@ -4882,7 +4879,7 @@
         <v>35</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>153</v>
@@ -4890,49 +4887,49 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2" s="8"/>
       <c r="G2" s="0" t="s">
         <v>165</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J2" s="12" t="n">
         <v>42940</v>
       </c>
       <c r="K2" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>165</v>
@@ -4943,27 +4940,27 @@
         <v>42940</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>165</v>
@@ -4974,54 +4971,54 @@
         <v>42940</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="8"/>
       <c r="G5" s="0" t="s">
         <v>165</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J5" s="12" t="n">
         <v>42950</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>165</v>
@@ -5032,27 +5029,27 @@
         <v>42950</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>165</v>
@@ -5063,27 +5060,27 @@
         <v>42950</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>165</v>
@@ -5094,45 +5091,45 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>165</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J9" s="12" t="n">
         <v>43011</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>165</v>
@@ -5145,22 +5142,22 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>165</v>
@@ -5173,13 +5170,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>6</v>
@@ -5190,7 +5187,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
@@ -5202,13 +5199,13 @@
         <v>8</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>165</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>